<commit_message>
prod. and proc. module
</commit_message>
<xml_diff>
--- a/data-input/estimated_variables.xlsx
+++ b/data-input/estimated_variables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12110" yWindow="-16320" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="12110" yWindow="-16320" windowWidth="10930" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="EstimatedVariables" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="182">
   <si>
     <t>Module</t>
   </si>
@@ -135,9 +135,6 @@
     <t>CFU</t>
   </si>
   <si>
-    <t>Load reduction factor after water washing (only water used in UK)</t>
-  </si>
-  <si>
     <t>Dampening factor for each successive wash</t>
   </si>
   <si>
@@ -396,9 +393,6 @@
     <t>Percentage of load increase due to cross-contamination between carcasses during evisceration</t>
   </si>
   <si>
-    <t>Percentage of load reduction after air pre-chilling (only washing technique used in UK)</t>
-  </si>
-  <si>
     <t>What fraction of the raw product represents the final processed product?</t>
   </si>
   <si>
@@ -432,9 +426,6 @@
     <t>F_df</t>
   </si>
   <si>
-    <t>F_wash</t>
-  </si>
-  <si>
     <t>F_wash_adj</t>
   </si>
   <si>
@@ -480,18 +471,12 @@
     <t>Black et al. (2015)</t>
   </si>
   <si>
-    <t>Bucher et al. (2012)</t>
-  </si>
-  <si>
     <t>Collineau et al. (2020)</t>
   </si>
   <si>
     <t>Robé et al. (2019)</t>
   </si>
   <si>
-    <t>Belluco et al. (2016)</t>
-  </si>
-  <si>
     <t>Thomas et al. (2020)</t>
   </si>
   <si>
@@ -504,9 +489,6 @@
     <t>Biglia et al. (2018); Evans and Redmond (2016); EcoSure (2007)</t>
   </si>
   <si>
-    <t>Huijbers et al. (2014); Daniel (2020)</t>
-  </si>
-  <si>
     <t>FAO/WHO (2002)</t>
   </si>
   <si>
@@ -514,9 +496,6 @@
   </si>
   <si>
     <t>FAO/WHO (2009)</t>
-  </si>
-  <si>
-    <t>Ewers et al. (2012)</t>
   </si>
   <si>
     <r>
@@ -585,10 +564,34 @@
     <t>Beta parameter used to describe cross-contamination between carcasses</t>
   </si>
   <si>
-    <t>Hinton et al. (1996)</t>
-  </si>
-  <si>
     <t>log10CFU</t>
+  </si>
+  <si>
+    <t>Faverjon et al. (2022)</t>
+  </si>
+  <si>
+    <t>F_wash_IOBW</t>
+  </si>
+  <si>
+    <t>Load reduction factor after water Inside Outside Bird Washing (IOBW)</t>
+  </si>
+  <si>
+    <t>Load reduction factor after Post Evisceration washing (PE)</t>
+  </si>
+  <si>
+    <t>F_wash_PE</t>
+  </si>
+  <si>
+    <t>wash_type</t>
+  </si>
+  <si>
+    <t>FIA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type of washing used: IOBW if &gt; 0,625 else IOBW+PE </t>
+  </si>
+  <si>
+    <t>Proportion of cells remaining after air chilling (AC)</t>
   </si>
 </sst>
 </file>
@@ -722,7 +725,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -766,11 +769,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -786,7 +798,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -795,7 +806,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -820,6 +830,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1139,10 +1155,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P58"/>
+  <dimension ref="A1:P60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1150,7 +1166,7 @@
     <col min="1" max="1" width="19.1796875" customWidth="1"/>
     <col min="2" max="2" width="13.54296875" customWidth="1"/>
     <col min="3" max="3" width="18.6328125" customWidth="1"/>
-    <col min="4" max="4" width="64.81640625" customWidth="1"/>
+    <col min="4" max="4" width="73.54296875" customWidth="1"/>
     <col min="5" max="5" width="11.7265625" customWidth="1"/>
     <col min="6" max="6" width="14.7265625" customWidth="1"/>
     <col min="7" max="7" width="10.36328125" customWidth="1"/>
@@ -1165,7 +1181,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>1</v>
@@ -1180,7 +1196,7 @@
         <v>3</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H1" s="8" t="s">
         <v>7</v>
@@ -1189,48 +1205,48 @@
         <v>8</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L1" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="O1" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="P1" s="8" t="s">
         <v>67</v>
-      </c>
-      <c r="M1" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="N1" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="O1" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="P1" s="8" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" s="36" t="s">
         <v>102</v>
       </c>
-      <c r="C2" s="38" t="s">
+      <c r="D2" s="37" t="s">
         <v>103</v>
       </c>
-      <c r="D2" s="39" t="s">
-        <v>104</v>
-      </c>
-      <c r="E2" s="38" t="s">
-        <v>110</v>
+      <c r="E2" s="36" t="s">
+        <v>109</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -1243,34 +1259,34 @@
         <v>164</v>
       </c>
       <c r="N2" s="2"/>
-      <c r="O2" s="37" t="s">
-        <v>156</v>
+      <c r="O2" s="3" t="s">
+        <v>173</v>
       </c>
       <c r="P2" s="7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="C3" s="38" t="s">
-        <v>162</v>
-      </c>
-      <c r="D3" s="39" t="s">
-        <v>164</v>
-      </c>
-      <c r="E3" s="38" t="s">
-        <v>110</v>
+      <c r="B3" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="C3" s="36" t="s">
+        <v>155</v>
+      </c>
+      <c r="D3" s="37" t="s">
+        <v>157</v>
+      </c>
+      <c r="E3" s="36" t="s">
+        <v>109</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
@@ -1281,8 +1297,8 @@
       </c>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
-      <c r="O3" s="37" t="s">
-        <v>149</v>
+      <c r="O3" s="35" t="s">
+        <v>145</v>
       </c>
       <c r="P3" s="4"/>
     </row>
@@ -1290,23 +1306,23 @@
       <c r="A4" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="C4" s="38" t="s">
-        <v>163</v>
-      </c>
-      <c r="D4" s="39" t="s">
-        <v>165</v>
-      </c>
-      <c r="E4" s="38" t="s">
-        <v>110</v>
+      <c r="B4" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4" s="36" t="s">
+        <v>156</v>
+      </c>
+      <c r="D4" s="37" t="s">
+        <v>158</v>
+      </c>
+      <c r="E4" s="36" t="s">
+        <v>109</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
@@ -1317,8 +1333,8 @@
       </c>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
-      <c r="O4" s="37" t="s">
-        <v>149</v>
+      <c r="O4" s="35" t="s">
+        <v>145</v>
       </c>
       <c r="P4" s="4"/>
     </row>
@@ -1326,65 +1342,65 @@
       <c r="A5" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="C5" s="38" t="s">
+      <c r="B5" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="C5" s="36" t="s">
+        <v>104</v>
+      </c>
+      <c r="D5" s="37" t="s">
         <v>105</v>
       </c>
-      <c r="D5" s="39" t="s">
-        <v>106</v>
-      </c>
-      <c r="E5" s="38" t="s">
-        <v>110</v>
+      <c r="E5" s="36" t="s">
+        <v>109</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H5" s="2">
-        <v>0.12</v>
+        <v>0.157</v>
       </c>
       <c r="I5" s="2">
-        <v>0.89</v>
+        <v>0.314</v>
       </c>
       <c r="J5" s="2">
-        <v>0.42</v>
+        <v>0.23499999999999999</v>
       </c>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
-      <c r="O5" s="37" t="s">
-        <v>160</v>
+      <c r="O5" s="35" t="s">
+        <v>145</v>
       </c>
       <c r="P5" s="4" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="C6" s="38" t="s">
+      <c r="B6" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="C6" s="36" t="s">
+        <v>106</v>
+      </c>
+      <c r="D6" s="37" t="s">
         <v>107</v>
       </c>
-      <c r="D6" s="39" t="s">
+      <c r="E6" s="36" t="s">
         <v>108</v>
-      </c>
-      <c r="E6" s="38" t="s">
-        <v>109</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H6" s="2">
         <v>18000</v>
@@ -1399,34 +1415,34 @@
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
-      <c r="O6" s="37" t="s">
-        <v>147</v>
+      <c r="O6" s="35" t="s">
+        <v>144</v>
       </c>
       <c r="P6" s="4" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="C7" s="38" t="s">
-        <v>130</v>
-      </c>
-      <c r="D7" s="39" t="s">
-        <v>139</v>
-      </c>
-      <c r="E7" s="38" t="s">
+      <c r="B7" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="C7" s="36" t="s">
+        <v>128</v>
+      </c>
+      <c r="D7" s="37" t="s">
+        <v>136</v>
+      </c>
+      <c r="E7" s="36" t="s">
         <v>23</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H7" s="2">
         <v>0</v>
@@ -1439,8 +1455,8 @@
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
-      <c r="O7" s="3" t="s">
-        <v>148</v>
+      <c r="O7" s="35" t="s">
+        <v>145</v>
       </c>
       <c r="P7" s="4"/>
     </row>
@@ -1448,23 +1464,23 @@
       <c r="A8" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="C8" s="38" t="s">
+      <c r="B8" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="C8" s="36" t="s">
+        <v>110</v>
+      </c>
+      <c r="D8" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="D8" s="39" t="s">
-        <v>112</v>
-      </c>
-      <c r="E8" s="38" t="s">
-        <v>138</v>
+      <c r="E8" s="36" t="s">
+        <v>135</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
@@ -1475,32 +1491,32 @@
       </c>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
-      <c r="O8" s="37" t="s">
-        <v>149</v>
+      <c r="O8" s="35" t="s">
+        <v>145</v>
       </c>
       <c r="P8" s="4"/>
     </row>
     <row r="9" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="36" t="s">
-        <v>101</v>
-      </c>
-      <c r="C9" s="40" t="s">
-        <v>115</v>
-      </c>
-      <c r="D9" s="41" t="s">
-        <v>113</v>
-      </c>
-      <c r="E9" s="40" t="s">
+      <c r="B9" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="C9" s="38" t="s">
+        <v>114</v>
+      </c>
+      <c r="D9" s="39" t="s">
+        <v>112</v>
+      </c>
+      <c r="E9" s="38" t="s">
         <v>32</v>
       </c>
       <c r="F9" s="9" t="s">
         <v>5</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H9" s="9">
         <v>4.4000000000000004</v>
@@ -1516,33 +1532,33 @@
       <c r="M9" s="9"/>
       <c r="N9" s="9"/>
       <c r="O9" s="10" t="s">
-        <v>168</v>
-      </c>
-      <c r="P9" s="48" t="s">
-        <v>169</v>
+        <v>161</v>
+      </c>
+      <c r="P9" s="46" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="C10" s="42" t="s">
-        <v>123</v>
-      </c>
-      <c r="D10" s="39" t="s">
+      <c r="B10" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" s="40" t="s">
+        <v>121</v>
+      </c>
+      <c r="D10" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="38" t="s">
+      <c r="E10" s="36" t="s">
         <v>12</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>5</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H10" s="2">
         <v>1</v>
@@ -1558,7 +1574,7 @@
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
       <c r="O10" s="2" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="P10" s="2"/>
     </row>
@@ -1566,23 +1582,23 @@
       <c r="A11" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="C11" s="38" t="s">
+      <c r="B11" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="39" t="s">
+      <c r="D11" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="38" t="s">
+      <c r="E11" s="36" t="s">
         <v>15</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>6</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H11" s="2">
         <v>0</v>
@@ -1596,7 +1612,7 @@
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
       <c r="O11" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="P11" s="2"/>
     </row>
@@ -1604,23 +1620,23 @@
       <c r="A12" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="C12" s="43" t="s">
+      <c r="B12" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="C12" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="44" t="s">
+      <c r="D12" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="43" t="s">
-        <v>63</v>
+      <c r="E12" s="41" t="s">
+        <v>62</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>4</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H12" s="5">
         <v>1.5</v>
@@ -1635,8 +1651,8 @@
       <c r="L12" s="5"/>
       <c r="M12" s="5"/>
       <c r="N12" s="5"/>
-      <c r="O12" s="5" t="s">
-        <v>148</v>
+      <c r="O12" s="2" t="s">
+        <v>145</v>
       </c>
       <c r="P12" s="5"/>
     </row>
@@ -1644,23 +1660,23 @@
       <c r="A13" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="22" t="s">
-        <v>101</v>
-      </c>
-      <c r="C13" s="46" t="s">
-        <v>166</v>
-      </c>
-      <c r="D13" s="39" t="s">
-        <v>170</v>
-      </c>
-      <c r="E13" s="38" t="s">
-        <v>136</v>
+      <c r="B13" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C13" s="44" t="s">
+        <v>159</v>
+      </c>
+      <c r="D13" s="37" t="s">
+        <v>163</v>
+      </c>
+      <c r="E13" s="36" t="s">
+        <v>133</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
@@ -1672,7 +1688,7 @@
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
       <c r="O13" s="2" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="P13" s="2"/>
     </row>
@@ -1680,23 +1696,23 @@
       <c r="A14" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="22" t="s">
-        <v>101</v>
-      </c>
-      <c r="C14" s="46" t="s">
-        <v>167</v>
-      </c>
-      <c r="D14" s="39" t="s">
-        <v>171</v>
-      </c>
-      <c r="E14" s="38" t="s">
-        <v>136</v>
+      <c r="B14" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C14" s="44" t="s">
+        <v>160</v>
+      </c>
+      <c r="D14" s="37" t="s">
+        <v>164</v>
+      </c>
+      <c r="E14" s="36" t="s">
+        <v>133</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
@@ -1708,7 +1724,7 @@
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
       <c r="O14" s="2" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="P14" s="2"/>
     </row>
@@ -1716,23 +1732,23 @@
       <c r="A15" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="22" t="s">
-        <v>101</v>
-      </c>
-      <c r="C15" s="46" t="s">
-        <v>141</v>
-      </c>
-      <c r="D15" s="47" t="s">
-        <v>142</v>
-      </c>
-      <c r="E15" s="38" t="s">
-        <v>136</v>
+      <c r="B15" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C15" s="44" t="s">
+        <v>138</v>
+      </c>
+      <c r="D15" s="45" t="s">
+        <v>139</v>
+      </c>
+      <c r="E15" s="36" t="s">
+        <v>133</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
@@ -1746,33 +1762,33 @@
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
       <c r="O15" s="3" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="22" t="s">
-        <v>101</v>
-      </c>
-      <c r="C16" s="38" t="s">
-        <v>175</v>
-      </c>
-      <c r="D16" s="39" t="s">
-        <v>177</v>
-      </c>
-      <c r="E16" s="38" t="s">
+      <c r="B16" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C16" s="36" t="s">
+        <v>168</v>
+      </c>
+      <c r="D16" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="E16" s="36" t="s">
         <v>10</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
@@ -1784,7 +1800,7 @@
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
       <c r="O16" s="3" t="s">
-        <v>179</v>
+        <v>145</v>
       </c>
       <c r="P16" s="2"/>
     </row>
@@ -1792,23 +1808,23 @@
       <c r="A17" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="22" t="s">
-        <v>101</v>
-      </c>
-      <c r="C17" s="38" t="s">
-        <v>176</v>
-      </c>
-      <c r="D17" s="39" t="s">
-        <v>178</v>
-      </c>
-      <c r="E17" s="38" t="s">
+      <c r="B17" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C17" s="36" t="s">
+        <v>169</v>
+      </c>
+      <c r="D17" s="37" t="s">
+        <v>171</v>
+      </c>
+      <c r="E17" s="36" t="s">
         <v>10</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
@@ -1820,7 +1836,7 @@
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
       <c r="O17" s="3" t="s">
-        <v>179</v>
+        <v>145</v>
       </c>
       <c r="P17" s="2"/>
     </row>
@@ -1828,23 +1844,23 @@
       <c r="A18" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="22" t="s">
-        <v>101</v>
-      </c>
-      <c r="C18" s="38" t="s">
-        <v>131</v>
-      </c>
-      <c r="D18" s="39" t="s">
+      <c r="B18" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C18" s="36" t="s">
+        <v>129</v>
+      </c>
+      <c r="D18" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="E18" s="38" t="s">
-        <v>180</v>
+      <c r="E18" s="36" t="s">
+        <v>172</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>5</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H18" s="3">
         <v>-4.01</v>
@@ -1860,33 +1876,33 @@
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
       <c r="O18" s="3" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="22" t="s">
-        <v>101</v>
-      </c>
-      <c r="C19" s="38" t="s">
+      <c r="B19" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C19" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="D19" s="39" t="s">
+      <c r="D19" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="E19" s="38" t="s">
+      <c r="E19" s="36" t="s">
         <v>23</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
@@ -1898,7 +1914,7 @@
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
       <c r="O19" s="3" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="P19" s="2"/>
     </row>
@@ -1906,23 +1922,23 @@
       <c r="A20" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="22" t="s">
-        <v>101</v>
-      </c>
-      <c r="C20" s="38" t="s">
+      <c r="B20" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C20" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="D20" s="39" t="s">
-        <v>143</v>
-      </c>
-      <c r="E20" s="38" t="s">
+      <c r="D20" s="37" t="s">
+        <v>140</v>
+      </c>
+      <c r="E20" s="36" t="s">
         <v>23</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H20" s="2">
         <v>0</v>
@@ -1940,7 +1956,7 @@
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
       <c r="O20" s="3" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="P20" s="3"/>
     </row>
@@ -1948,23 +1964,23 @@
       <c r="A21" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="22" t="s">
-        <v>101</v>
-      </c>
-      <c r="C21" s="38" t="s">
+      <c r="B21" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C21" s="36" t="s">
+        <v>81</v>
+      </c>
+      <c r="D21" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="D21" s="39" t="s">
+      <c r="E21" s="36" t="s">
         <v>83</v>
-      </c>
-      <c r="E21" s="38" t="s">
-        <v>84</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>5</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H21" s="2">
         <v>0.54</v>
@@ -1979,31 +1995,31 @@
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
-      <c r="O21" s="37" t="s">
-        <v>150</v>
+      <c r="O21" s="35" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A22" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="22" t="s">
-        <v>101</v>
-      </c>
-      <c r="C22" s="38" t="s">
+      <c r="B22" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C22" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="D22" s="39" t="s">
+      <c r="D22" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="E22" s="38" t="s">
+      <c r="E22" s="36" t="s">
         <v>23</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>5</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H22" s="2">
         <v>0.03</v>
@@ -2019,7 +2035,7 @@
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
       <c r="O22" s="3" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="P22" s="2"/>
     </row>
@@ -2027,23 +2043,23 @@
       <c r="A23" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="22" t="s">
-        <v>101</v>
-      </c>
-      <c r="C23" s="38" t="s">
+      <c r="B23" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C23" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="D23" s="39" t="s">
-        <v>119</v>
-      </c>
-      <c r="E23" s="38" t="s">
-        <v>35</v>
+      <c r="D23" s="37" t="s">
+        <v>118</v>
+      </c>
+      <c r="E23" s="36" t="s">
+        <v>34</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>5</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H23" s="3">
         <v>0.06</v>
@@ -2058,1114 +2074,1209 @@
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
-      <c r="O23" s="3"/>
-      <c r="P23" s="2"/>
+      <c r="O23" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="P23" s="46" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A24" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B24" s="22" t="s">
-        <v>101</v>
-      </c>
-      <c r="C24" s="38" t="s">
-        <v>132</v>
-      </c>
-      <c r="D24" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="E24" s="38" t="s">
-        <v>88</v>
+      <c r="B24" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C24" s="36" t="s">
+        <v>178</v>
+      </c>
+      <c r="D24" s="37" t="s">
+        <v>180</v>
+      </c>
+      <c r="E24" s="36" t="s">
+        <v>10</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="H24" s="2">
-        <v>-0.96</v>
-      </c>
-      <c r="I24" s="2">
-        <v>-0.28000000000000003</v>
-      </c>
-      <c r="J24" s="2">
-        <v>-0.62</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="H24" s="3">
+        <v>0</v>
+      </c>
+      <c r="I24" s="3">
+        <v>1</v>
+      </c>
+      <c r="J24" s="3"/>
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
       <c r="O24" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="P24" s="2"/>
+        <v>179</v>
+      </c>
+      <c r="P24" s="46"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A25" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="22" t="s">
-        <v>101</v>
-      </c>
-      <c r="C25" s="38" t="s">
-        <v>133</v>
-      </c>
-      <c r="D25" s="39" t="s">
-        <v>34</v>
-      </c>
-      <c r="E25" s="38" t="s">
-        <v>10</v>
+      <c r="B25" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C25" s="36" t="s">
+        <v>174</v>
+      </c>
+      <c r="D25" s="37" t="s">
+        <v>175</v>
+      </c>
+      <c r="E25" s="36" t="s">
+        <v>172</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H25" s="2">
-        <v>0</v>
+        <v>-1.29</v>
       </c>
       <c r="I25" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="J25" s="2"/>
+        <v>-0.55000000000000004</v>
+      </c>
+      <c r="J25" s="2">
+        <v>-0.92</v>
+      </c>
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
-      <c r="O25" s="37" t="s">
-        <v>149</v>
-      </c>
-      <c r="P25" s="2"/>
+      <c r="O25" s="35" t="s">
+        <v>145</v>
+      </c>
+      <c r="P25" s="2" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A26" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B26" s="22" t="s">
-        <v>101</v>
-      </c>
-      <c r="C26" s="38" t="s">
-        <v>134</v>
-      </c>
-      <c r="D26" s="39" t="s">
-        <v>120</v>
-      </c>
-      <c r="E26" s="38" t="s">
-        <v>35</v>
+      <c r="B26" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C26" s="36" t="s">
+        <v>177</v>
+      </c>
+      <c r="D26" s="37" t="s">
+        <v>176</v>
+      </c>
+      <c r="E26" s="36" t="s">
+        <v>172</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>65</v>
+        <v>5</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
+        <v>79</v>
+      </c>
+      <c r="H26" s="2">
+        <v>-1.28</v>
+      </c>
+      <c r="I26" s="2">
+        <v>-1.06</v>
+      </c>
+      <c r="J26" s="2">
+        <v>-1.17</v>
+      </c>
       <c r="K26" s="2"/>
-      <c r="L26" s="2">
-        <v>-0.126</v>
-      </c>
+      <c r="L26" s="2"/>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
-      <c r="O26" s="37"/>
-      <c r="P26" s="2"/>
+      <c r="O26" s="35" t="s">
+        <v>145</v>
+      </c>
+      <c r="P26" s="2" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A27" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B27" s="22" t="s">
-        <v>101</v>
-      </c>
-      <c r="C27" s="38" t="s">
-        <v>116</v>
-      </c>
-      <c r="D27" s="39" t="s">
-        <v>87</v>
-      </c>
-      <c r="E27" s="38" t="s">
+      <c r="B27" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C27" s="36" t="s">
+        <v>130</v>
+      </c>
+      <c r="D27" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="E27" s="36" t="s">
         <v>10</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="H27" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="I27" s="3">
-        <v>1</v>
-      </c>
-      <c r="J27" s="3">
-        <v>0.02</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="H27" s="2">
+        <v>0</v>
+      </c>
+      <c r="I27" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="J27" s="2"/>
       <c r="K27" s="2"/>
-      <c r="L27" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="L27" s="2"/>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
-      <c r="O27" s="37"/>
+      <c r="O27" s="35" t="s">
+        <v>145</v>
+      </c>
       <c r="P27" s="2"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A28" s="14" t="s">
+      <c r="A28" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B28" s="23" t="s">
-        <v>101</v>
-      </c>
-      <c r="C28" s="40" t="s">
-        <v>85</v>
-      </c>
-      <c r="D28" s="41" t="s">
-        <v>86</v>
-      </c>
-      <c r="E28" s="40" t="s">
-        <v>23</v>
-      </c>
-      <c r="F28" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="G28" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="H28" s="9"/>
-      <c r="I28" s="9"/>
-      <c r="J28" s="9"/>
-      <c r="K28" s="9"/>
-      <c r="L28" s="9">
-        <v>1</v>
-      </c>
-      <c r="M28" s="9">
-        <v>3.15</v>
-      </c>
-      <c r="N28" s="9"/>
-      <c r="O28" s="10"/>
-      <c r="P28" s="9"/>
+      <c r="B28" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C28" s="36" t="s">
+        <v>131</v>
+      </c>
+      <c r="D28" s="37" t="s">
+        <v>181</v>
+      </c>
+      <c r="E28" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H28" s="3">
+        <v>5.1050499999999999E-2</v>
+      </c>
+      <c r="I28" s="3">
+        <v>0.31045600000000001</v>
+      </c>
+      <c r="J28" s="3">
+        <v>0.12589249999999999</v>
+      </c>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+      <c r="O28" s="35" t="s">
+        <v>145</v>
+      </c>
+      <c r="P28" s="2"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A29" s="13" t="s">
         <v>19</v>
       </c>
       <c r="B29" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="C29" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="D29" s="39" t="s">
-        <v>26</v>
-      </c>
-      <c r="E29" s="38" t="s">
-        <v>23</v>
+        <v>100</v>
+      </c>
+      <c r="C29" s="36" t="s">
+        <v>115</v>
+      </c>
+      <c r="D29" s="37" t="s">
+        <v>86</v>
+      </c>
+      <c r="E29" s="36" t="s">
+        <v>10</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="H29" s="2">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="I29" s="2">
-        <v>0.23</v>
+        <v>4</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H29" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="I29" s="3">
+        <v>1</v>
       </c>
       <c r="J29" s="3">
-        <v>0.18</v>
+        <v>0.02</v>
       </c>
       <c r="K29" s="2"/>
-      <c r="L29" s="2"/>
+      <c r="L29" s="2">
+        <v>0.5</v>
+      </c>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
-      <c r="O29" s="37" t="s">
-        <v>149</v>
+      <c r="O29" s="35" t="s">
+        <v>145</v>
       </c>
       <c r="P29" s="2"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A30" s="13" t="s">
+      <c r="A30" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B30" s="21" t="s">
-        <v>67</v>
+      <c r="B30" s="22" t="s">
+        <v>100</v>
       </c>
       <c r="C30" s="38" t="s">
+        <v>84</v>
+      </c>
+      <c r="D30" s="39" t="s">
+        <v>85</v>
+      </c>
+      <c r="E30" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="G30" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
+      <c r="K30" s="9"/>
+      <c r="L30" s="9">
+        <v>1</v>
+      </c>
+      <c r="M30" s="9">
+        <v>3.15</v>
+      </c>
+      <c r="N30" s="9"/>
+      <c r="O30" s="35" t="s">
+        <v>145</v>
+      </c>
+      <c r="P30" s="9"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A31" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="C31" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="D31" s="37" t="s">
+        <v>26</v>
+      </c>
+      <c r="E31" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="H31" s="2">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="I31" s="2">
+        <v>0.23</v>
+      </c>
+      <c r="J31" s="3">
+        <v>0.18</v>
+      </c>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="35" t="s">
+        <v>145</v>
+      </c>
+      <c r="P31" s="2"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A32" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B32" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="C32" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="D30" s="39" t="s">
+      <c r="D32" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="E30" s="38" t="s">
+      <c r="E32" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="F32" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G30" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="H30" s="3">
+      <c r="G32" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="H32" s="3">
         <v>1</v>
       </c>
-      <c r="I30" s="3">
+      <c r="I32" s="3">
         <v>10</v>
       </c>
-      <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
-      <c r="L30" s="2"/>
-      <c r="M30" s="2"/>
-      <c r="N30" s="2"/>
-      <c r="O30" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="P30" s="2"/>
-    </row>
-    <row r="31" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B31" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="C31" s="43" t="s">
-        <v>124</v>
-      </c>
-      <c r="D31" s="44" t="s">
-        <v>121</v>
-      </c>
-      <c r="E31" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="G31" s="6"/>
-      <c r="H31" s="5"/>
-      <c r="I31" s="5"/>
-      <c r="J31" s="6"/>
-      <c r="K31" s="5"/>
-      <c r="L31" s="5">
-        <v>0.25</v>
-      </c>
-      <c r="M31" s="5"/>
-      <c r="N31" s="5"/>
-      <c r="O31" s="6"/>
-      <c r="P31" s="5" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A32" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="B32" s="29" t="s">
-        <v>101</v>
-      </c>
-      <c r="C32" s="38" t="s">
-        <v>89</v>
-      </c>
-      <c r="D32" s="39" t="s">
-        <v>90</v>
-      </c>
-      <c r="E32" s="38" t="s">
-        <v>44</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
-      <c r="L32" s="2">
-        <v>7</v>
-      </c>
+      <c r="L32" s="2"/>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
-      <c r="O32" s="3"/>
+      <c r="O32" s="3" t="s">
+        <v>145</v>
+      </c>
       <c r="P32" s="2"/>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A33" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="B33" s="29" t="s">
-        <v>101</v>
-      </c>
-      <c r="C33" s="38" t="s">
-        <v>91</v>
-      </c>
-      <c r="D33" s="39" t="s">
-        <v>92</v>
-      </c>
-      <c r="E33" s="38" t="s">
-        <v>44</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="H33" s="2">
+    <row r="33" spans="1:16" s="51" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A33" s="47" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33" s="48" t="s">
+        <v>66</v>
+      </c>
+      <c r="C33" s="49" t="s">
+        <v>122</v>
+      </c>
+      <c r="D33" s="50" t="s">
+        <v>119</v>
+      </c>
+      <c r="E33" s="49" t="s">
+        <v>34</v>
+      </c>
+      <c r="F33" s="51" t="s">
+        <v>64</v>
+      </c>
+      <c r="G33" s="52" t="s">
+        <v>79</v>
+      </c>
+      <c r="J33" s="52"/>
+      <c r="L33" s="51">
+        <v>0.25</v>
+      </c>
+      <c r="O33" s="52" t="s">
+        <v>173</v>
+      </c>
+      <c r="P33" s="51" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="I33" s="2">
-        <v>40</v>
-      </c>
-      <c r="J33" s="2">
-        <v>37</v>
-      </c>
-      <c r="K33" s="2"/>
-      <c r="L33" s="2"/>
-      <c r="M33" s="2"/>
-      <c r="N33" s="2"/>
-      <c r="O33" s="3"/>
-      <c r="P33" s="2"/>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A34" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="B34" s="29" t="s">
-        <v>101</v>
-      </c>
-      <c r="C34" s="38" t="s">
-        <v>135</v>
-      </c>
-      <c r="D34" s="39" t="s">
-        <v>93</v>
-      </c>
-      <c r="E34" s="38" t="s">
+      <c r="B34" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="C34" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="F34" s="3" t="s">
-        <v>5</v>
+      <c r="D34" s="37" t="s">
+        <v>89</v>
+      </c>
+      <c r="E34" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="H34" s="2">
-        <v>-0.3</v>
-      </c>
-      <c r="I34" s="2">
-        <v>-0.1</v>
-      </c>
-      <c r="J34" s="2">
-        <v>-0.2</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
       <c r="K34" s="2"/>
-      <c r="L34" s="2"/>
+      <c r="L34" s="2">
+        <v>7</v>
+      </c>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
-      <c r="O34" s="3" t="s">
-        <v>152</v>
-      </c>
+      <c r="O34" s="3"/>
       <c r="P34" s="2"/>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A35" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="B35" s="29" t="s">
-        <v>101</v>
-      </c>
-      <c r="C35" s="38" t="s">
-        <v>94</v>
-      </c>
-      <c r="D35" s="39" t="s">
-        <v>95</v>
-      </c>
-      <c r="E35" s="38" t="s">
-        <v>96</v>
+      <c r="A35" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="C35" s="36" t="s">
+        <v>90</v>
+      </c>
+      <c r="D35" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="E35" s="36" t="s">
+        <v>43</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>65</v>
+        <v>4</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
-      <c r="J35" s="2"/>
+        <v>79</v>
+      </c>
+      <c r="H35" s="2">
+        <v>35</v>
+      </c>
+      <c r="I35" s="2">
+        <v>40</v>
+      </c>
+      <c r="J35" s="2">
+        <v>37</v>
+      </c>
       <c r="K35" s="2"/>
-      <c r="L35" s="2">
-        <v>0.47</v>
-      </c>
+      <c r="L35" s="2"/>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
-      <c r="O35" s="2" t="s">
-        <v>153</v>
-      </c>
+      <c r="O35" s="3"/>
       <c r="P35" s="2"/>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A36" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="B36" s="29" t="s">
-        <v>101</v>
-      </c>
-      <c r="C36" s="40" t="s">
-        <v>125</v>
-      </c>
-      <c r="D36" s="41" t="s">
-        <v>97</v>
-      </c>
-      <c r="E36" s="40" t="s">
-        <v>84</v>
-      </c>
-      <c r="F36" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="G36" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="H36" s="9"/>
-      <c r="I36" s="9"/>
-      <c r="J36" s="9"/>
-      <c r="K36" s="9"/>
-      <c r="L36" s="9">
-        <v>123000</v>
-      </c>
-      <c r="M36" s="9"/>
-      <c r="N36" s="9"/>
-      <c r="O36" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="P36" s="9"/>
+      <c r="A36" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="C36" s="36" t="s">
+        <v>132</v>
+      </c>
+      <c r="D36" s="37" t="s">
+        <v>92</v>
+      </c>
+      <c r="E36" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H36" s="2">
+        <v>-0.3</v>
+      </c>
+      <c r="I36" s="2">
+        <v>-0.1</v>
+      </c>
+      <c r="J36" s="2">
+        <v>-0.2</v>
+      </c>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+      <c r="N36" s="2"/>
+      <c r="O36" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="P36" s="2"/>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A37" s="16" t="s">
-        <v>36</v>
+      <c r="A37" s="15" t="s">
+        <v>35</v>
       </c>
       <c r="B37" s="27" t="s">
-        <v>67</v>
-      </c>
-      <c r="C37" s="38" t="s">
-        <v>37</v>
-      </c>
-      <c r="D37" s="39" t="s">
-        <v>122</v>
-      </c>
-      <c r="E37" s="38" t="s">
-        <v>12</v>
+        <v>100</v>
+      </c>
+      <c r="C37" s="36" t="s">
+        <v>93</v>
+      </c>
+      <c r="D37" s="37" t="s">
+        <v>94</v>
+      </c>
+      <c r="E37" s="36" t="s">
+        <v>95</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
-      <c r="J37" s="2">
-        <v>1495.3</v>
-      </c>
-      <c r="K37" s="2">
-        <v>303.39999999999998</v>
-      </c>
-      <c r="L37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2">
+        <v>0.47</v>
+      </c>
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
+      <c r="O37" s="2" t="s">
+        <v>148</v>
+      </c>
       <c r="P37" s="2"/>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A38" s="16" t="s">
+      <c r="A38" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B38" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="C38" s="38" t="s">
+        <v>123</v>
+      </c>
+      <c r="D38" s="39" t="s">
+        <v>96</v>
+      </c>
+      <c r="E38" s="38" t="s">
+        <v>83</v>
+      </c>
+      <c r="F38" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="G38" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="H38" s="9"/>
+      <c r="I38" s="9"/>
+      <c r="J38" s="9"/>
+      <c r="K38" s="9"/>
+      <c r="L38" s="9">
+        <v>123000</v>
+      </c>
+      <c r="M38" s="9"/>
+      <c r="N38" s="9"/>
+      <c r="O38" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="P38" s="9"/>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A39" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B39" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="C39" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="B38" s="27" t="s">
-        <v>67</v>
-      </c>
-      <c r="C38" s="38" t="s">
-        <v>126</v>
-      </c>
-      <c r="D38" s="39" t="s">
-        <v>38</v>
-      </c>
-      <c r="E38" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G38" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="H38" s="2">
-        <v>0.6</v>
-      </c>
-      <c r="I38" s="2">
-        <v>0.65</v>
-      </c>
-      <c r="J38" s="2"/>
-      <c r="K38" s="2"/>
-      <c r="L38" s="2"/>
-      <c r="M38" s="2"/>
-      <c r="N38" s="2"/>
-      <c r="O38" t="s">
-        <v>154</v>
-      </c>
-      <c r="P38" s="2"/>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A39" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="B39" s="27" t="s">
-        <v>67</v>
-      </c>
-      <c r="C39" s="38" t="s">
-        <v>39</v>
-      </c>
-      <c r="D39" s="39" t="s">
-        <v>40</v>
-      </c>
-      <c r="E39" s="38" t="s">
-        <v>41</v>
+      <c r="D39" s="37" t="s">
+        <v>120</v>
+      </c>
+      <c r="E39" s="36" t="s">
+        <v>12</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G39" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="H39" s="2">
-        <v>1</v>
-      </c>
-      <c r="I39" s="2">
-        <v>7</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
       <c r="J39" s="2">
-        <v>3</v>
-      </c>
-      <c r="K39" s="2"/>
+        <v>1495.3</v>
+      </c>
+      <c r="K39" s="2">
+        <v>303.39999999999998</v>
+      </c>
       <c r="L39" s="2"/>
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
-      <c r="O39" s="2"/>
       <c r="P39" s="2"/>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A40" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="B40" s="27" t="s">
-        <v>67</v>
-      </c>
-      <c r="C40" s="38" t="s">
-        <v>42</v>
-      </c>
-      <c r="D40" s="39" t="s">
-        <v>43</v>
-      </c>
-      <c r="E40" s="38" t="s">
-        <v>44</v>
+      <c r="A40" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B40" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="C40" s="36" t="s">
+        <v>124</v>
+      </c>
+      <c r="D40" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="E40" s="36" t="s">
+        <v>34</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>74</v>
+        <v>6</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H40" s="2">
-        <v>-6.67</v>
+        <v>0.6</v>
       </c>
       <c r="I40" s="2">
-        <v>19.440000000000001</v>
-      </c>
-      <c r="J40" s="2">
-        <v>3.3332999999999999</v>
-      </c>
+        <v>0.65</v>
+      </c>
+      <c r="J40" s="2"/>
       <c r="K40" s="2"/>
-      <c r="L40" s="2">
-        <v>2.6623000000000001</v>
-      </c>
+      <c r="L40" s="2"/>
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
-      <c r="O40" s="2"/>
+      <c r="O40" t="s">
+        <v>149</v>
+      </c>
       <c r="P40" s="2"/>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A41" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="B41" s="27" t="s">
-        <v>67</v>
-      </c>
-      <c r="C41" s="38" t="s">
-        <v>47</v>
-      </c>
-      <c r="D41" s="39" t="s">
-        <v>48</v>
-      </c>
-      <c r="E41" s="38" t="s">
-        <v>44</v>
+      <c r="A41" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B41" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="C41" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="D41" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="E41" s="36" t="s">
+        <v>40</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>118</v>
+        <v>5</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="H41" s="3">
-        <v>-5.56</v>
-      </c>
-      <c r="I41" s="3">
-        <v>20</v>
-      </c>
-      <c r="J41" s="2"/>
+        <v>79</v>
+      </c>
+      <c r="H41" s="2">
+        <v>1</v>
+      </c>
+      <c r="I41" s="2">
+        <v>7</v>
+      </c>
+      <c r="J41" s="2">
+        <v>3</v>
+      </c>
       <c r="K41" s="2"/>
-      <c r="L41" s="3">
-        <v>29.370999999999999</v>
-      </c>
-      <c r="M41" s="2">
-        <v>16.763000000000002</v>
-      </c>
-      <c r="N41" s="2">
-        <v>-22.914999999999999</v>
-      </c>
-      <c r="O41" t="s">
-        <v>149</v>
-      </c>
+      <c r="L41" s="2"/>
+      <c r="M41" s="2"/>
+      <c r="N41" s="2"/>
+      <c r="O41" s="2"/>
       <c r="P41" s="2"/>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A42" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="B42" s="27" t="s">
-        <v>67</v>
-      </c>
-      <c r="C42" s="38" t="s">
-        <v>45</v>
-      </c>
-      <c r="D42" s="39" t="s">
-        <v>144</v>
-      </c>
-      <c r="E42" s="38" t="s">
-        <v>46</v>
+      <c r="A42" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B42" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="C42" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="D42" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="E42" s="36" t="s">
+        <v>43</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="G42" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
+      <c r="H42" s="2">
+        <v>-6.67</v>
+      </c>
+      <c r="I42" s="2">
+        <v>19.440000000000001</v>
+      </c>
       <c r="J42" s="2">
-        <v>69.599999999999994</v>
-      </c>
-      <c r="K42" s="2">
-        <v>0.438</v>
-      </c>
-      <c r="L42" s="2"/>
+        <v>3.3332999999999999</v>
+      </c>
+      <c r="K42" s="2"/>
+      <c r="L42" s="2">
+        <v>2.6623000000000001</v>
+      </c>
       <c r="M42" s="2"/>
       <c r="N42" s="2"/>
-      <c r="O42" t="s">
-        <v>149</v>
-      </c>
+      <c r="O42" s="2"/>
       <c r="P42" s="2"/>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A43" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="B43" s="27" t="s">
-        <v>67</v>
-      </c>
-      <c r="C43" s="38" t="s">
-        <v>49</v>
-      </c>
-      <c r="D43" s="39" t="s">
-        <v>145</v>
-      </c>
-      <c r="E43" s="38" t="s">
-        <v>41</v>
+      <c r="A43" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B43" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="C43" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="D43" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="E43" s="36" t="s">
+        <v>43</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>70</v>
+        <v>117</v>
       </c>
       <c r="G43" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="H43" s="2"/>
-      <c r="I43" s="2"/>
-      <c r="J43" s="2">
+      <c r="H43" s="3">
+        <v>-5.56</v>
+      </c>
+      <c r="I43" s="3">
+        <v>20</v>
+      </c>
+      <c r="J43" s="2"/>
+      <c r="K43" s="2"/>
+      <c r="L43" s="3">
+        <v>29.370999999999999</v>
+      </c>
+      <c r="M43" s="2">
+        <v>16.763000000000002</v>
+      </c>
+      <c r="N43" s="2">
+        <v>-22.914999999999999</v>
+      </c>
+      <c r="O43" t="s">
+        <v>145</v>
+      </c>
+      <c r="P43" s="2"/>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A44" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B44" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="C44" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="D44" s="37" t="s">
+        <v>141</v>
+      </c>
+      <c r="E44" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2">
+        <v>69.599999999999994</v>
+      </c>
+      <c r="K44" s="2">
+        <v>0.438</v>
+      </c>
+      <c r="L44" s="2"/>
+      <c r="M44" s="2"/>
+      <c r="N44" s="2"/>
+      <c r="O44" t="s">
+        <v>145</v>
+      </c>
+      <c r="P44" s="2"/>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A45" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B45" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="C45" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="D45" s="37" t="s">
+        <v>142</v>
+      </c>
+      <c r="E45" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2">
         <v>2.2000000000000002</v>
       </c>
-      <c r="K43" s="2">
+      <c r="K45" s="2">
         <v>2.0299999999999999E-2</v>
       </c>
-      <c r="L43" s="2"/>
-      <c r="M43" s="2"/>
-      <c r="N43" s="2"/>
-      <c r="O43" t="s">
-        <v>149</v>
-      </c>
-      <c r="P43" s="2"/>
-    </row>
-    <row r="44" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="B44" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="C44" s="43" t="s">
-        <v>50</v>
-      </c>
-      <c r="D44" s="44" t="s">
-        <v>51</v>
-      </c>
-      <c r="E44" s="43" t="s">
-        <v>44</v>
-      </c>
-      <c r="F44" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="G44" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="H44" s="5">
-        <v>-4.4400000000000004</v>
-      </c>
-      <c r="I44" s="5">
-        <v>16.11</v>
-      </c>
-      <c r="J44" s="5">
-        <v>5.3</v>
-      </c>
-      <c r="K44" s="5"/>
-      <c r="L44" s="6">
-        <v>2.2965</v>
-      </c>
-      <c r="M44" s="5"/>
-      <c r="N44" s="5"/>
-      <c r="O44" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="P44" s="5"/>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A45" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="B45" s="30" t="s">
-        <v>101</v>
-      </c>
-      <c r="C45" s="38" t="s">
-        <v>98</v>
-      </c>
-      <c r="D45" s="39" t="s">
-        <v>99</v>
-      </c>
-      <c r="E45" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G45" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="H45" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="I45" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="J45" s="3">
-        <v>0.16</v>
-      </c>
-      <c r="K45" s="2"/>
       <c r="L45" s="2"/>
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
       <c r="O45" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="P45" s="2"/>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A46" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="B46" s="31" t="s">
-        <v>101</v>
-      </c>
-      <c r="C46" s="40" t="s">
-        <v>127</v>
-      </c>
-      <c r="D46" s="41" t="s">
-        <v>128</v>
-      </c>
-      <c r="E46" s="45" t="s">
+    <row r="46" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A46" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="F46" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="G46" s="10" t="s">
+      <c r="B46" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="C46" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="D46" s="42" t="s">
+        <v>50</v>
+      </c>
+      <c r="E46" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="G46" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="H46" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="I46" s="10">
+      <c r="H46" s="5">
+        <v>-4.4400000000000004</v>
+      </c>
+      <c r="I46" s="5">
+        <v>16.11</v>
+      </c>
+      <c r="J46" s="5">
+        <v>5.3</v>
+      </c>
+      <c r="K46" s="5"/>
+      <c r="L46" s="6">
+        <v>2.2965</v>
+      </c>
+      <c r="M46" s="5"/>
+      <c r="N46" s="5"/>
+      <c r="O46" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="P46" s="5"/>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A47" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B47" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="C47" s="36" t="s">
+        <v>97</v>
+      </c>
+      <c r="D47" s="37" t="s">
+        <v>98</v>
+      </c>
+      <c r="E47" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="H47" s="2">
         <v>0.1</v>
       </c>
-      <c r="J46" s="9"/>
-      <c r="K46" s="9"/>
-      <c r="L46" s="9"/>
-      <c r="M46" s="9"/>
-      <c r="N46" s="9"/>
-      <c r="O46" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="P46" s="9"/>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A47" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="B47" s="32" t="s">
-        <v>67</v>
-      </c>
-      <c r="C47" s="38" t="s">
-        <v>53</v>
-      </c>
-      <c r="D47" s="39" t="s">
-        <v>146</v>
-      </c>
-      <c r="E47" s="38" t="s">
-        <v>23</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="G47" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="H47" s="2"/>
-      <c r="I47" s="2"/>
-      <c r="J47" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="K47" s="2">
-        <v>2.1199999999999999E-3</v>
-      </c>
+      <c r="I47" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="J47" s="3">
+        <v>0.16</v>
+      </c>
+      <c r="K47" s="2"/>
       <c r="L47" s="2"/>
       <c r="M47" s="2"/>
       <c r="N47" s="2"/>
-      <c r="O47" s="2" t="s">
-        <v>149</v>
+      <c r="O47" t="s">
+        <v>151</v>
       </c>
       <c r="P47" s="2"/>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A48" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B48" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="C48" s="38" t="s">
+        <v>125</v>
+      </c>
+      <c r="D48" s="39" t="s">
+        <v>126</v>
+      </c>
+      <c r="E48" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="F48" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G48" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="H48" s="10">
+        <v>0.01</v>
+      </c>
+      <c r="I48" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="J48" s="9"/>
+      <c r="K48" s="9"/>
+      <c r="L48" s="9"/>
+      <c r="M48" s="9"/>
+      <c r="N48" s="9"/>
+      <c r="O48" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="P48" s="9"/>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A49" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B49" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="C49" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="B48" s="32" t="s">
-        <v>67</v>
-      </c>
-      <c r="C48" s="38" t="s">
-        <v>54</v>
-      </c>
-      <c r="D48" s="39" t="s">
-        <v>55</v>
-      </c>
-      <c r="E48" s="38" t="s">
-        <v>46</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G48" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="H48" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="I48" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="J48" s="3">
-        <v>1</v>
-      </c>
-      <c r="K48" s="2"/>
-      <c r="L48" s="2"/>
-      <c r="M48" s="2"/>
-      <c r="N48" s="2"/>
-      <c r="O48" t="s">
-        <v>157</v>
-      </c>
-      <c r="P48" s="2"/>
-    </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A49" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="B49" s="32" t="s">
-        <v>67</v>
-      </c>
-      <c r="C49" s="38" t="s">
-        <v>56</v>
-      </c>
-      <c r="D49" s="39" t="s">
-        <v>57</v>
-      </c>
-      <c r="E49" s="38" t="s">
-        <v>44</v>
+      <c r="D49" s="37" t="s">
+        <v>143</v>
+      </c>
+      <c r="E49" s="36" t="s">
+        <v>23</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>4</v>
+        <v>69</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="H49" s="2">
-        <v>60</v>
-      </c>
-      <c r="I49" s="2">
-        <v>65</v>
-      </c>
-      <c r="J49" s="3">
-        <v>64</v>
-      </c>
-      <c r="K49" s="2"/>
+        <v>79</v>
+      </c>
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
+      <c r="J49" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="K49" s="2">
+        <v>2.1199999999999999E-3</v>
+      </c>
       <c r="L49" s="2"/>
       <c r="M49" s="2"/>
       <c r="N49" s="2"/>
-      <c r="O49" t="s">
-        <v>157</v>
+      <c r="O49" s="2" t="s">
+        <v>145</v>
       </c>
       <c r="P49" s="2"/>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A50" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="B50" s="32" t="s">
-        <v>67</v>
-      </c>
-      <c r="C50" s="38" t="s">
-        <v>58</v>
-      </c>
-      <c r="D50" s="39" t="s">
-        <v>59</v>
-      </c>
-      <c r="E50" s="38" t="s">
-        <v>23</v>
+      <c r="A50" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B50" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="C50" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="D50" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="E50" s="36" t="s">
+        <v>45</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="H50" s="3">
-        <v>0.38</v>
+        <v>79</v>
+      </c>
+      <c r="H50" s="2">
+        <v>0.5</v>
       </c>
       <c r="I50" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="J50" s="3">
         <v>1</v>
       </c>
-      <c r="J50" s="2"/>
       <c r="K50" s="2"/>
       <c r="L50" s="2"/>
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
       <c r="O50" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="P50" s="2"/>
     </row>
-    <row r="51" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A51" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="B51" s="33" t="s">
-        <v>67</v>
-      </c>
-      <c r="C51" s="43" t="s">
-        <v>61</v>
-      </c>
-      <c r="D51" s="44" t="s">
-        <v>62</v>
-      </c>
-      <c r="E51" s="43" t="s">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A51" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B51" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="C51" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="D51" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="E51" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="H51" s="2">
         <v>60</v>
       </c>
-      <c r="F51" s="5" t="s">
+      <c r="I51" s="2">
+        <v>65</v>
+      </c>
+      <c r="J51" s="3">
+        <v>64</v>
+      </c>
+      <c r="K51" s="2"/>
+      <c r="L51" s="2"/>
+      <c r="M51" s="2"/>
+      <c r="N51" s="2"/>
+      <c r="O51" t="s">
+        <v>151</v>
+      </c>
+      <c r="P51" s="2"/>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A52" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B52" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="C52" s="36" t="s">
+        <v>57</v>
+      </c>
+      <c r="D52" s="37" t="s">
+        <v>58</v>
+      </c>
+      <c r="E52" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="F52" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G51" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="H51" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="I51" s="5">
-        <v>1.5</v>
-      </c>
-      <c r="J51" s="5"/>
-      <c r="K51" s="5"/>
-      <c r="L51" s="5"/>
-      <c r="M51" s="5"/>
-      <c r="N51" s="5"/>
-      <c r="O51" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="P51" s="5"/>
-    </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="G52" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="H52" s="3">
+        <v>0.38</v>
+      </c>
+      <c r="I52" s="2">
+        <v>1</v>
+      </c>
+      <c r="J52" s="2"/>
+      <c r="K52" s="2"/>
       <c r="L52" s="2"/>
       <c r="M52" s="2"/>
       <c r="N52" s="2"/>
-    </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="K53" s="2"/>
+      <c r="O52" t="s">
+        <v>152</v>
+      </c>
+      <c r="P52" s="2"/>
+    </row>
+    <row r="53" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A53" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B53" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="C53" s="41" t="s">
+        <v>60</v>
+      </c>
+      <c r="D53" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="E53" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="F53" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G53" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="H53" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="I53" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="J53" s="5"/>
+      <c r="K53" s="5"/>
+      <c r="L53" s="5"/>
+      <c r="M53" s="5"/>
+      <c r="N53" s="5"/>
+      <c r="O53" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="P53" s="5"/>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="K54" s="2"/>
+      <c r="L54" s="2"/>
+      <c r="M54" s="2"/>
+      <c r="N54" s="2"/>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.35">
       <c r="K55" s="2"/>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.35">
       <c r="K56" s="2"/>
-      <c r="O56" s="2"/>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.35">
       <c r="K57" s="2"/>
-      <c r="O57" s="2"/>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="K58" s="2"/>
       <c r="O58" s="2"/>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="K59" s="2"/>
+      <c r="O59" s="2"/>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="O60" s="2"/>
     </row>
   </sheetData>
   <dataValidations xWindow="721" yWindow="594" count="10">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Standard deviation" prompt="Enter the standard deviation of the mean of the probability distribution. This cell must be filled only when the selected probability distribution is &quot;Normal&quot;" sqref="K53:K57">
-      <formula1>I53</formula1>
-      <formula2>J53</formula2>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Standard deviation" prompt="Enter the standard deviation of the mean of the probability distribution. This cell must be filled only when the selected probability distribution is &quot;Normal&quot;" sqref="K55:K59">
+      <formula1>I55</formula1>
+      <formula2>J55</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMean" error="Something is wrong. Please enter a value between the minimum and maximum values" promptTitle="Mean" prompt="Enter the most likely value (or mean value) of the probability distribution. This cell must remain empty when the selected probability distribution is &quot;Uniform&quot;_x000a_" sqref="O57">
-      <formula1>K57</formula1>
-      <formula2>L57</formula2>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMean" error="Something is wrong. Please enter a value between the minimum and maximum values" promptTitle="Mean" prompt="Enter the most likely value (or mean value) of the probability distribution. This cell must remain empty when the selected probability distribution is &quot;Uniform&quot;_x000a_" sqref="O59">
+      <formula1>K59</formula1>
+      <formula2>L59</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Standard deviation" prompt="Enter the standard deviation of the mean of the probability distribution. This cell must be filled only when the selected probability distribution is &quot;Normal&quot; or &quot;LogNormal&quot;" sqref="K21:K51 K2:K19">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Standard deviation" prompt="Enter the standard deviation of the mean of the probability distribution. This cell must be filled only when the selected probability distribution is &quot;Normal&quot; or &quot;LogNormal&quot;" sqref="K2:K19 K21:K53">
       <formula1>I2</formula1>
       <formula2>J2</formula2>
     </dataValidation>
@@ -3173,19 +3284,19 @@
       <formula1>O20</formula1>
       <formula2>#REF!</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Other" prompt="Enter the parameter of the probability distribution not covered by the previous columns. Examples: second shape parameter of the Beta distribution_x000a_" sqref="M2:M51"/>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMax" error="Something is wrong. Are you sure the value you entered is the maximal value?" promptTitle="Maximum" prompt="Enter the maximal value of the probability distribution. This cell can be also used to define the upper bound of truncated distributions." sqref="I2:I51">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Other" prompt="Enter the parameter of the probability distribution not covered by the previous columns. Examples: second shape parameter of the Beta distribution_x000a_" sqref="M2:M53"/>
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMax" error="Something is wrong. Are you sure the value you entered is the maximal value?" promptTitle="Maximum" prompt="Enter the maximal value of the probability distribution. This cell can be also used to define the upper bound of truncated distributions." sqref="I2:I53">
       <formula1>H2</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMean" error="Something is wrong. Please enter a value between the minimum and maximum values" promptTitle="Mean" prompt="Enter the most likely value (or mean value) of the probability distribution. _x000a_" sqref="J2:J51">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMean" error="Something is wrong. Please enter a value between the minimum and maximum values" promptTitle="Mean" prompt="Enter the most likely value (or mean value) of the probability distribution. _x000a_" sqref="J2:J53">
       <formula1>H2</formula1>
       <formula2>I2</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Other" prompt="Enter the parameter of the probability distribution, which had not been covered by the previous columns. Examples: value of the &quot;Point estimate&quot; variable, parameters of &quot;Poisson&quot; or &quot;NegBin&quot; (negative binomial) distributions" sqref="L2:L51"/>
-    <dataValidation type="decimal" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMin" error="Something is wrong. Are you sure the value you entered is the minimum value?" promptTitle="Minimum" prompt="Enter Minimal value of the probability distribution. This cell can be also used to defined the lower bound of truncated distributions." sqref="H2:H51">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Other" prompt="Enter the parameter of the probability distribution, which had not been covered by the previous columns. Examples: value of the &quot;Point estimate&quot; variable, parameters of &quot;Poisson&quot; or &quot;NegBin&quot; (negative binomial) distributions" sqref="L2:L53"/>
+    <dataValidation type="decimal" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMin" error="Something is wrong. Are you sure the value you entered is the minimum value?" promptTitle="Minimum" prompt="Enter Minimal value of the probability distribution. This cell can be also used to defined the lower bound of truncated distributions." sqref="H2:H53">
       <formula1>I2</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Other3" prompt="Enter the parameter of the probability distribution not covered by the previous columns. Examples: shift parameter of the shifted log logistic distribution_x000a_" sqref="N2:N51"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Other3" prompt="Enter the parameter of the probability distribution not covered by the previous columns. Examples: shift parameter of the shifted log logistic distribution_x000a_" sqref="N2:N53"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3196,13 +3307,13 @@
           <x14:formula1>
             <xm:f>ListItem!$B$3:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G51</xm:sqref>
+          <xm:sqref>G2:G53</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Distribution" prompt="Select a probability distribution">
           <x14:formula1>
             <xm:f>ListItem!$A$2:$A$16</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F51</xm:sqref>
+          <xm:sqref>F2:F53</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3228,23 +3339,23 @@
         <v>3</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C1" s="4"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C3" s="2"/>
     </row>
@@ -3253,13 +3364,13 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -3280,63 +3391,63 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>

</xml_diff>

<commit_message>
home prep. module + doc.
</commit_message>
<xml_diff>
--- a/data-input/estimated_variables.xlsx
+++ b/data-input/estimated_variables.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="189">
   <si>
     <t>Module</t>
   </si>
@@ -357,9 +357,6 @@
     <t>Bacteria concentration in the barn environment</t>
   </si>
   <si>
-    <t>CFU/kg of feces</t>
-  </si>
-  <si>
     <t>Prevalence</t>
   </si>
   <si>
@@ -465,22 +462,7 @@
     <t>Mean probability of undercooking to occur</t>
   </si>
   <si>
-    <t>Black et al. (2015)</t>
-  </si>
-  <si>
     <t>Collineau et al. (2020)</t>
-  </si>
-  <si>
-    <t>Robé et al. (2019)</t>
-  </si>
-  <si>
-    <t>FAO/WHO (2002)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Collineau et al. (2020); Bruhn (2014) </t>
-  </si>
-  <si>
-    <t>FAO/WHO (2009)</t>
   </si>
   <si>
     <r>
@@ -516,9 +498,6 @@
     <t>C_prod.max</t>
   </si>
   <si>
-    <t>Berrang et Northcutt (2005)</t>
-  </si>
-  <si>
     <t>à vérifier</t>
   </si>
   <si>
@@ -528,9 +507,6 @@
     <t>Maximum incoming load on the carcass to have a 100% prevalence</t>
   </si>
   <si>
-    <t>Althaus et al. (2017)</t>
-  </si>
-  <si>
     <t>assumption: scalding type is soft</t>
   </si>
   <si>
@@ -619,6 +595,24 @@
   </si>
   <si>
     <t>F_freezer</t>
+  </si>
+  <si>
+    <t>V_dil_car</t>
+  </si>
+  <si>
+    <t>Volume of fluid diluting for a whole carcass</t>
+  </si>
+  <si>
+    <t>D_value_alpha</t>
+  </si>
+  <si>
+    <t>Intercept term for D-value computation</t>
+  </si>
+  <si>
+    <t>D_value_beta</t>
+  </si>
+  <si>
+    <t>Coefficient term for D-value computation</t>
   </si>
 </sst>
 </file>
@@ -1183,10 +1177,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P66"/>
+  <dimension ref="A1:P69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C31" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="L37" sqref="L37"/>
+    <sheetView tabSelected="1" topLeftCell="F10" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1194,7 +1188,7 @@
     <col min="1" max="1" width="19.1796875" customWidth="1"/>
     <col min="2" max="2" width="13.54296875" customWidth="1"/>
     <col min="3" max="3" width="18.6328125" customWidth="1"/>
-    <col min="4" max="4" width="29.54296875" customWidth="1"/>
+    <col min="4" max="4" width="36.6328125" customWidth="1"/>
     <col min="5" max="5" width="11.7265625" customWidth="1"/>
     <col min="6" max="6" width="14.7265625" customWidth="1"/>
     <col min="7" max="7" width="10.36328125" customWidth="1"/>
@@ -1233,7 +1227,7 @@
         <v>8</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K1" s="8" t="s">
         <v>67</v>
@@ -1245,7 +1239,7 @@
         <v>74</v>
       </c>
       <c r="N1" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="O1" s="8" t="s">
         <v>62</v>
@@ -1268,7 +1262,7 @@
         <v>102</v>
       </c>
       <c r="E2" s="36" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>71</v>
@@ -1288,10 +1282,10 @@
       </c>
       <c r="N2" s="2"/>
       <c r="O2" s="3" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="P2" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -1302,13 +1296,13 @@
         <v>99</v>
       </c>
       <c r="C3" s="36" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="D3" s="37" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="E3" s="36" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>63</v>
@@ -1326,7 +1320,7 @@
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
       <c r="O3" s="35" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="P3" s="4"/>
     </row>
@@ -1338,13 +1332,13 @@
         <v>99</v>
       </c>
       <c r="C4" s="36" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D4" s="37" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="E4" s="36" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>63</v>
@@ -1362,7 +1356,7 @@
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
       <c r="O4" s="35" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="P4" s="4"/>
     </row>
@@ -1380,7 +1374,7 @@
         <v>104</v>
       </c>
       <c r="E5" s="36" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>4</v>
@@ -1402,10 +1396,10 @@
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="O5" s="35" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="P5" s="4" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -1422,7 +1416,7 @@
         <v>106</v>
       </c>
       <c r="E6" s="36" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>4</v>
@@ -1431,23 +1425,23 @@
         <v>78</v>
       </c>
       <c r="H6" s="2">
-        <v>18000</v>
+        <v>18000000</v>
       </c>
       <c r="I6" s="2">
-        <v>5400000</v>
+        <v>5400000000</v>
       </c>
       <c r="J6" s="2">
-        <v>1100000</v>
+        <v>1100000000</v>
       </c>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
-      <c r="O6" s="35" t="s">
+      <c r="O6" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="P6" s="4" t="s">
         <v>143</v>
-      </c>
-      <c r="P6" s="4" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -1458,10 +1452,10 @@
         <v>99</v>
       </c>
       <c r="C7" s="36" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D7" s="37" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E7" s="36" t="s">
         <v>23</v>
@@ -1484,7 +1478,7 @@
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
       <c r="O7" s="35" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="P7" s="4"/>
     </row>
@@ -1496,13 +1490,13 @@
         <v>99</v>
       </c>
       <c r="C8" s="36" t="s">
+        <v>108</v>
+      </c>
+      <c r="D8" s="37" t="s">
         <v>109</v>
       </c>
-      <c r="D8" s="37" t="s">
-        <v>110</v>
-      </c>
       <c r="E8" s="36" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>63</v>
@@ -1520,7 +1514,7 @@
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
       <c r="O8" s="35" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="P8" s="4"/>
     </row>
@@ -1532,10 +1526,10 @@
         <v>99</v>
       </c>
       <c r="C9" s="38" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D9" s="39" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E9" s="38" t="s">
         <v>32</v>
@@ -1559,11 +1553,11 @@
       <c r="L9" s="9"/>
       <c r="M9" s="9"/>
       <c r="N9" s="9"/>
-      <c r="O9" s="10" t="s">
-        <v>156</v>
+      <c r="O9" s="3" t="s">
+        <v>160</v>
       </c>
       <c r="P9" s="46" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.35">
@@ -1574,7 +1568,7 @@
         <v>65</v>
       </c>
       <c r="C10" s="40" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D10" s="37" t="s">
         <v>11</v>
@@ -1602,7 +1596,7 @@
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
       <c r="O10" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="P10" s="2"/>
     </row>
@@ -1640,7 +1634,7 @@
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
       <c r="O11" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="P11" s="2"/>
     </row>
@@ -1680,7 +1674,7 @@
       <c r="M12" s="5"/>
       <c r="N12" s="5"/>
       <c r="O12" s="5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="P12" s="5"/>
     </row>
@@ -1692,13 +1686,13 @@
         <v>99</v>
       </c>
       <c r="C13" s="44" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="D13" s="37" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="E13" s="36" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>63</v>
@@ -1716,7 +1710,7 @@
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
       <c r="O13" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="P13" s="2"/>
     </row>
@@ -1728,13 +1722,13 @@
         <v>99</v>
       </c>
       <c r="C14" s="44" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="D14" s="37" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="E14" s="36" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>63</v>
@@ -1752,7 +1746,7 @@
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
       <c r="O14" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="P14" s="2"/>
     </row>
@@ -1764,13 +1758,13 @@
         <v>99</v>
       </c>
       <c r="C15" s="44" t="s">
+        <v>136</v>
+      </c>
+      <c r="D15" s="45" t="s">
         <v>137</v>
       </c>
-      <c r="D15" s="45" t="s">
-        <v>138</v>
-      </c>
       <c r="E15" s="36" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>68</v>
@@ -1793,7 +1787,7 @@
         <v>160</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.35">
@@ -1804,10 +1798,10 @@
         <v>99</v>
       </c>
       <c r="C16" s="36" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="D16" s="37" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="E16" s="36" t="s">
         <v>10</v>
@@ -1828,7 +1822,7 @@
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
       <c r="O16" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="P16" s="2"/>
     </row>
@@ -1840,10 +1834,10 @@
         <v>99</v>
       </c>
       <c r="C17" s="36" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="D17" s="37" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="E17" s="36" t="s">
         <v>10</v>
@@ -1864,7 +1858,7 @@
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
       <c r="O17" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="P17" s="2"/>
     </row>
@@ -1876,13 +1870,13 @@
         <v>99</v>
       </c>
       <c r="C18" s="36" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D18" s="37" t="s">
         <v>20</v>
       </c>
       <c r="E18" s="36" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>5</v>
@@ -1904,10 +1898,10 @@
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
       <c r="O18" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.35">
@@ -1942,7 +1936,7 @@
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
       <c r="O19" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="P19" s="2"/>
     </row>
@@ -1957,7 +1951,7 @@
         <v>24</v>
       </c>
       <c r="D20" s="37" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E20" s="36" t="s">
         <v>23</v>
@@ -1984,7 +1978,7 @@
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
       <c r="O20" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="P20" s="3"/>
     </row>
@@ -2023,8 +2017,8 @@
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
-      <c r="O21" s="35" t="s">
-        <v>145</v>
+      <c r="O21" s="3" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.35">
@@ -2063,7 +2057,7 @@
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
       <c r="O22" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="P22" s="2"/>
     </row>
@@ -2078,7 +2072,7 @@
         <v>31</v>
       </c>
       <c r="D23" s="37" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E23" s="36" t="s">
         <v>34</v>
@@ -2103,10 +2097,10 @@
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
       <c r="O23" s="3" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="P23" s="7" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.35">
@@ -2117,10 +2111,10 @@
         <v>99</v>
       </c>
       <c r="C24" s="36" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="D24" s="37" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="E24" s="36" t="s">
         <v>10</v>
@@ -2143,7 +2137,7 @@
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
       <c r="O24" s="3" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="P24" s="7"/>
     </row>
@@ -2155,13 +2149,13 @@
         <v>99</v>
       </c>
       <c r="C25" s="36" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="D25" s="37" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="E25" s="36" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>5</v>
@@ -2183,10 +2177,10 @@
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
       <c r="O25" s="35" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="P25" s="2" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.35">
@@ -2197,13 +2191,13 @@
         <v>99</v>
       </c>
       <c r="C26" s="36" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="D26" s="37" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="E26" s="36" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>5</v>
@@ -2225,10 +2219,10 @@
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
       <c r="O26" s="35" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="P26" s="2" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.35">
@@ -2239,7 +2233,7 @@
         <v>99</v>
       </c>
       <c r="C27" s="36" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D27" s="37" t="s">
         <v>33</v>
@@ -2265,7 +2259,7 @@
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
       <c r="O27" s="35" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="P27" s="2"/>
     </row>
@@ -2277,10 +2271,10 @@
         <v>99</v>
       </c>
       <c r="C28" s="36" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D28" s="37" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="E28" s="36" t="s">
         <v>34</v>
@@ -2305,7 +2299,7 @@
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
       <c r="O28" s="35" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="P28" s="2"/>
     </row>
@@ -2317,7 +2311,7 @@
         <v>99</v>
       </c>
       <c r="C29" s="36" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D29" s="37" t="s">
         <v>85</v>
@@ -2347,7 +2341,7 @@
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
       <c r="O29" s="35" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="P29" s="2"/>
     </row>
@@ -2385,7 +2379,7 @@
       </c>
       <c r="N30" s="9"/>
       <c r="O30" s="51" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="P30" s="9"/>
     </row>
@@ -2425,7 +2419,7 @@
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
       <c r="O31" s="35" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="P31" s="2"/>
     </row>
@@ -2463,7 +2457,7 @@
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
       <c r="O32" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="P32" s="2"/>
     </row>
@@ -2475,10 +2469,10 @@
         <v>65</v>
       </c>
       <c r="C33" s="49" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D33" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E33" s="49" t="s">
         <v>34</v>
@@ -2494,10 +2488,10 @@
         <v>0.25</v>
       </c>
       <c r="O33" s="6" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="P33" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.35">
@@ -2532,7 +2526,7 @@
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
       <c r="O34" s="3" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="P34" s="2"/>
     </row>
@@ -2572,7 +2566,7 @@
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
       <c r="O35" s="3" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="P35" s="2"/>
     </row>
@@ -2584,7 +2578,7 @@
         <v>99</v>
       </c>
       <c r="C36" s="36" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D36" s="37" t="s">
         <v>91</v>
@@ -2612,7 +2606,7 @@
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
       <c r="O36" s="3" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="P36" s="2"/>
     </row>
@@ -2624,10 +2618,10 @@
         <v>99</v>
       </c>
       <c r="C37" s="36" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="D37" s="37" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="E37" s="36" t="s">
         <v>34</v>
@@ -2647,7 +2641,7 @@
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
       <c r="O37" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="P37" s="2"/>
     </row>
@@ -2683,7 +2677,7 @@
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
       <c r="O38" s="3" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="P38" s="2"/>
     </row>
@@ -2695,7 +2689,7 @@
         <v>99</v>
       </c>
       <c r="C39" s="38" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D39" s="39" t="s">
         <v>95</v>
@@ -2719,7 +2713,7 @@
       <c r="M39" s="9"/>
       <c r="N39" s="9"/>
       <c r="O39" s="10" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="P39" s="9"/>
     </row>
@@ -2731,10 +2725,10 @@
         <v>65</v>
       </c>
       <c r="C40" s="36" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="D40" s="37" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E40" s="36" t="s">
         <v>12</v>
@@ -2754,7 +2748,7 @@
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
       <c r="O40" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="P40" s="2"/>
     </row>
@@ -2766,10 +2760,10 @@
         <v>65</v>
       </c>
       <c r="C41" s="36" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="D41" s="37" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="E41" s="36" t="s">
         <v>12</v>
@@ -2789,7 +2783,7 @@
       <c r="M41" s="2"/>
       <c r="N41" s="2"/>
       <c r="O41" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="P41" s="2"/>
     </row>
@@ -2801,10 +2795,10 @@
         <v>65</v>
       </c>
       <c r="C42" s="36" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="D42" s="37" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="E42" s="36" t="s">
         <v>12</v>
@@ -2824,7 +2818,7 @@
       <c r="M42" s="2"/>
       <c r="N42" s="2"/>
       <c r="O42" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="P42" s="2"/>
     </row>
@@ -2836,10 +2830,10 @@
         <v>65</v>
       </c>
       <c r="C43" s="36" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="D43" s="37" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="E43" s="36" t="s">
         <v>12</v>
@@ -2859,7 +2853,7 @@
       <c r="M43" s="2"/>
       <c r="N43" s="2"/>
       <c r="O43" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="P43" s="2"/>
     </row>
@@ -2871,7 +2865,7 @@
         <v>65</v>
       </c>
       <c r="C44" s="36" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D44" s="37" t="s">
         <v>36</v>
@@ -2897,7 +2891,7 @@
       <c r="M44" s="2"/>
       <c r="N44" s="2"/>
       <c r="O44" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="P44" s="2"/>
     </row>
@@ -2937,7 +2931,7 @@
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
       <c r="O45" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="P45" s="2"/>
     </row>
@@ -2952,7 +2946,7 @@
         <v>43</v>
       </c>
       <c r="D46" s="37" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E46" s="36" t="s">
         <v>44</v>
@@ -2975,7 +2969,7 @@
       <c r="M46" s="2"/>
       <c r="N46" s="2"/>
       <c r="O46" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="P46" s="2"/>
     </row>
@@ -2990,7 +2984,7 @@
         <v>47</v>
       </c>
       <c r="D47" s="37" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E47" s="36" t="s">
         <v>39</v>
@@ -3013,7 +3007,7 @@
       <c r="M47" s="2"/>
       <c r="N47" s="2"/>
       <c r="O47" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="P47" s="2"/>
     </row>
@@ -3055,7 +3049,7 @@
       <c r="M48" s="2"/>
       <c r="N48" s="2"/>
       <c r="O48" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="P48" s="2"/>
     </row>
@@ -3076,7 +3070,7 @@
         <v>42</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G49" s="3" t="s">
         <v>79</v>
@@ -3099,7 +3093,7 @@
         <v>-22.914999999999999</v>
       </c>
       <c r="O49" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="P49" s="2"/>
     </row>
@@ -3141,7 +3135,7 @@
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
       <c r="O50" s="3" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="P50" s="2"/>
     </row>
@@ -3153,10 +3147,10 @@
         <v>65</v>
       </c>
       <c r="C51" s="52" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="D51" s="53" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="E51" s="36" t="s">
         <v>34</v>
@@ -3177,7 +3171,7 @@
       <c r="M51" s="2"/>
       <c r="N51" s="2"/>
       <c r="O51" s="2" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="P51" s="2"/>
     </row>
@@ -3189,10 +3183,10 @@
         <v>65</v>
       </c>
       <c r="C52" s="41" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="D52" s="42" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="E52" s="49" t="s">
         <v>34</v>
@@ -3213,7 +3207,7 @@
       <c r="M52" s="5"/>
       <c r="N52" s="5"/>
       <c r="O52" s="5" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="P52" s="5"/>
     </row>
@@ -3253,7 +3247,7 @@
       <c r="M53" s="2"/>
       <c r="N53" s="2"/>
       <c r="O53" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="P53" s="2"/>
     </row>
@@ -3265,10 +3259,10 @@
         <v>99</v>
       </c>
       <c r="C54" s="38" t="s">
+        <v>123</v>
+      </c>
+      <c r="D54" s="39" t="s">
         <v>124</v>
-      </c>
-      <c r="D54" s="39" t="s">
-        <v>125</v>
       </c>
       <c r="E54" s="43" t="s">
         <v>34</v>
@@ -3290,8 +3284,8 @@
       <c r="L54" s="9"/>
       <c r="M54" s="9"/>
       <c r="N54" s="9"/>
-      <c r="O54" s="9" t="s">
-        <v>144</v>
+      <c r="O54" t="s">
+        <v>142</v>
       </c>
       <c r="P54" s="9"/>
     </row>
@@ -3306,7 +3300,7 @@
         <v>51</v>
       </c>
       <c r="D55" s="37" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E55" s="36" t="s">
         <v>23</v>
@@ -3328,8 +3322,8 @@
       <c r="L55" s="2"/>
       <c r="M55" s="2"/>
       <c r="N55" s="2"/>
-      <c r="O55" s="2" t="s">
-        <v>144</v>
+      <c r="O55" t="s">
+        <v>142</v>
       </c>
       <c r="P55" s="2"/>
     </row>
@@ -3341,35 +3335,33 @@
         <v>65</v>
       </c>
       <c r="C56" s="36" t="s">
-        <v>52</v>
+        <v>183</v>
       </c>
       <c r="D56" s="37" t="s">
-        <v>53</v>
+        <v>184</v>
       </c>
       <c r="E56" s="36" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G56" s="3" t="s">
         <v>78</v>
       </c>
       <c r="H56" s="2">
-        <v>0.5</v>
+        <v>150</v>
       </c>
       <c r="I56" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="J56" s="3">
-        <v>1</v>
-      </c>
+        <v>250</v>
+      </c>
+      <c r="J56" s="3"/>
       <c r="K56" s="2"/>
       <c r="L56" s="2"/>
       <c r="M56" s="2"/>
       <c r="N56" s="2"/>
       <c r="O56" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="P56" s="2"/>
     </row>
@@ -3381,35 +3373,31 @@
         <v>65</v>
       </c>
       <c r="C57" s="36" t="s">
-        <v>54</v>
+        <v>185</v>
       </c>
       <c r="D57" s="37" t="s">
-        <v>55</v>
+        <v>186</v>
       </c>
       <c r="E57" s="36" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>4</v>
+        <v>63</v>
       </c>
       <c r="G57" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="H57" s="2">
-        <v>60</v>
-      </c>
-      <c r="I57" s="2">
-        <v>65</v>
-      </c>
-      <c r="J57" s="3">
-        <v>64</v>
-      </c>
+      <c r="H57" s="2"/>
+      <c r="I57" s="2"/>
+      <c r="J57" s="3"/>
       <c r="K57" s="2"/>
-      <c r="L57" s="2"/>
+      <c r="L57" s="2">
+        <v>8.58</v>
+      </c>
       <c r="M57" s="2"/>
       <c r="N57" s="2"/>
       <c r="O57" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="P57" s="2"/>
     </row>
@@ -3421,110 +3409,226 @@
         <v>65</v>
       </c>
       <c r="C58" s="36" t="s">
-        <v>56</v>
+        <v>187</v>
       </c>
       <c r="D58" s="37" t="s">
-        <v>57</v>
+        <v>188</v>
       </c>
       <c r="E58" s="36" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>6</v>
+        <v>63</v>
       </c>
       <c r="G58" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="H58" s="3">
-        <v>0.38</v>
-      </c>
-      <c r="I58" s="2">
-        <v>1</v>
-      </c>
-      <c r="J58" s="2"/>
+      <c r="H58" s="2"/>
+      <c r="I58" s="2"/>
+      <c r="J58" s="3"/>
       <c r="K58" s="2"/>
-      <c r="L58" s="2"/>
+      <c r="L58" s="2">
+        <v>-0.13900000000000001</v>
+      </c>
       <c r="M58" s="2"/>
       <c r="N58" s="2"/>
       <c r="O58" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="P58" s="2"/>
     </row>
-    <row r="59" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A59" s="19" t="s">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A59" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="B59" s="31" t="s">
+      <c r="B59" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="C59" s="41" t="s">
-        <v>59</v>
-      </c>
-      <c r="D59" s="42" t="s">
+      <c r="C59" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="D59" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="E59" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G59" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="H59" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="I59" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="J59" s="3">
+        <v>1</v>
+      </c>
+      <c r="K59" s="2"/>
+      <c r="L59" s="2"/>
+      <c r="M59" s="2"/>
+      <c r="N59" s="2"/>
+      <c r="O59" t="s">
+        <v>142</v>
+      </c>
+      <c r="P59" s="2"/>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A60" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B60" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="C60" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="D60" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="E60" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G60" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="H60" s="2">
         <v>60</v>
       </c>
-      <c r="E59" s="41" t="s">
-        <v>58</v>
-      </c>
-      <c r="F59" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G59" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="H59" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="I59" s="5">
-        <v>1.5</v>
-      </c>
-      <c r="J59" s="5"/>
-      <c r="K59" s="5"/>
-      <c r="L59" s="5"/>
-      <c r="M59" s="5"/>
-      <c r="N59" s="5"/>
-      <c r="O59" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="P59" s="5"/>
-    </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="I60" s="2">
+        <v>65</v>
+      </c>
+      <c r="J60" s="3">
+        <v>64</v>
+      </c>
+      <c r="K60" s="2"/>
       <c r="L60" s="2"/>
       <c r="M60" s="2"/>
       <c r="N60" s="2"/>
+      <c r="O60" t="s">
+        <v>142</v>
+      </c>
+      <c r="P60" s="2"/>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A61" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B61" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="C61" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="D61" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="E61" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G61" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="H61" s="3">
+        <v>0.38</v>
+      </c>
+      <c r="I61" s="2">
+        <v>1</v>
+      </c>
+      <c r="J61" s="2"/>
       <c r="K61" s="2"/>
-    </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="K62" s="2"/>
+      <c r="L61" s="2"/>
+      <c r="M61" s="2"/>
+      <c r="N61" s="2"/>
+      <c r="O61" t="s">
+        <v>142</v>
+      </c>
+      <c r="P61" s="2"/>
+    </row>
+    <row r="62" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A62" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B62" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="C62" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="D62" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="E62" s="41" t="s">
+        <v>58</v>
+      </c>
+      <c r="F62" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G62" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="H62" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="I62" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="J62" s="5"/>
+      <c r="K62" s="5"/>
+      <c r="L62" s="5"/>
+      <c r="M62" s="5"/>
+      <c r="N62" s="5"/>
+      <c r="O62" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="P62" s="5"/>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="K63" s="2"/>
+      <c r="L63" s="2"/>
+      <c r="M63" s="2"/>
+      <c r="N63" s="2"/>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.35">
       <c r="K64" s="2"/>
-      <c r="O64" s="2"/>
     </row>
     <row r="65" spans="11:15" x14ac:dyDescent="0.35">
       <c r="K65" s="2"/>
-      <c r="O65" s="2"/>
     </row>
     <row r="66" spans="11:15" x14ac:dyDescent="0.35">
-      <c r="O66" s="2"/>
+      <c r="K66" s="2"/>
+    </row>
+    <row r="67" spans="11:15" x14ac:dyDescent="0.35">
+      <c r="K67" s="2"/>
+      <c r="O67" s="2"/>
+    </row>
+    <row r="68" spans="11:15" x14ac:dyDescent="0.35">
+      <c r="K68" s="2"/>
+      <c r="O68" s="2"/>
+    </row>
+    <row r="69" spans="11:15" x14ac:dyDescent="0.35">
+      <c r="O69" s="2"/>
     </row>
   </sheetData>
   <dataValidations xWindow="721" yWindow="594" count="12">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Standard deviation" prompt="Enter the standard deviation of the mean of the probability distribution. This cell must be filled only when the selected probability distribution is &quot;Normal&quot;" sqref="K61:K65">
-      <formula1>I61</formula1>
-      <formula2>J61</formula2>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Standard deviation" prompt="Enter the standard deviation of the mean of the probability distribution. This cell must be filled only when the selected probability distribution is &quot;Normal&quot;" sqref="K64:K68">
+      <formula1>I64</formula1>
+      <formula2>J64</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMean" error="Something is wrong. Please enter a value between the minimum and maximum values" promptTitle="Mean" prompt="Enter the most likely value (or mean value) of the probability distribution. This cell must remain empty when the selected probability distribution is &quot;Uniform&quot;_x000a_" sqref="O65">
-      <formula1>K65</formula1>
-      <formula2>L65</formula2>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMean" error="Something is wrong. Please enter a value between the minimum and maximum values" promptTitle="Mean" prompt="Enter the most likely value (or mean value) of the probability distribution. This cell must remain empty when the selected probability distribution is &quot;Uniform&quot;_x000a_" sqref="O68">
+      <formula1>K68</formula1>
+      <formula2>L68</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Standard deviation" prompt="Enter the standard deviation of the mean of the probability distribution. This cell must be filled only when the selected probability distribution is &quot;Normal&quot; or &quot;LogNormal&quot;" sqref="K2:K19 K21:K59">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Standard deviation" prompt="Enter the standard deviation of the mean of the probability distribution. This cell must be filled only when the selected probability distribution is &quot;Normal&quot; or &quot;LogNormal&quot;" sqref="K2:K19 K21:K62">
       <formula1>I2</formula1>
       <formula2>J2</formula2>
     </dataValidation>
@@ -3532,20 +3636,20 @@
       <formula1>O20</formula1>
       <formula2>#REF!</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Other" prompt="Enter the parameter of the probability distribution not covered by the previous columns. Examples: second shape parameter of the Beta distribution_x000a_" sqref="M2:M59"/>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMax" error="Something is wrong. Are you sure the value you entered is the maximal value?" promptTitle="Maximum" prompt="Enter the maximal value of the probability distribution. This cell can be also used to define the upper bound of truncated distributions." sqref="I2:I59">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Other" prompt="Enter the parameter of the probability distribution not covered by the previous columns. Examples: second shape parameter of the Beta distribution_x000a_" sqref="M2:M62"/>
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMax" error="Something is wrong. Are you sure the value you entered is the maximal value?" promptTitle="Maximum" prompt="Enter the maximal value of the probability distribution. This cell can be also used to define the upper bound of truncated distributions." sqref="I2:I62">
       <formula1>H2</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Other" prompt="Enter the parameter of the probability distribution, which had not been covered by the previous columns. Examples: value of the &quot;Point estimate&quot; variable, parameters of &quot;Poisson&quot; or &quot;NegBin&quot; (negative binomial) distributions" sqref="L44:L59 L2:L36 L38:L39"/>
-    <dataValidation type="decimal" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMin" error="Something is wrong. Are you sure the value you entered is the minimum value?" promptTitle="Minimum" prompt="Enter Minimal value of the probability distribution. This cell can be also used to defined the lower bound of truncated distributions." sqref="H2:H59">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Other" prompt="Enter the parameter of the probability distribution, which had not been covered by the previous columns. Examples: value of the &quot;Point estimate&quot; variable, parameters of &quot;Poisson&quot; or &quot;NegBin&quot; (negative binomial) distributions" sqref="L38:L39 L2:L36 L44:L62"/>
+    <dataValidation type="decimal" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMin" error="Something is wrong. Are you sure the value you entered is the minimum value?" promptTitle="Minimum" prompt="Enter Minimal value of the probability distribution. This cell can be also used to defined the lower bound of truncated distributions." sqref="H2:H62">
       <formula1>I2</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Other3" prompt="Enter the parameter of the probability distribution not covered by the previous columns. Examples: shift parameter of the shifted log logistic distribution_x000a_" sqref="N2:N59"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Other3" prompt="Enter the parameter of the probability distribution not covered by the previous columns. Examples: shift parameter of the shifted log logistic distribution_x000a_" sqref="N2:N62"/>
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Standard deviation" prompt="Enter the standard deviation of the mean of the probability distribution. This cell must be filled only when the selected probability distribution is &quot;Normal&quot; or &quot;LogNormal&quot;" sqref="L41">
       <formula1>H41</formula1>
       <formula2>I41</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMean" error="Something is wrong. Please enter a value between the minimum and maximum values" promptTitle="Mean" prompt="Enter the most likely value (or mean value) of the probability distribution. _x000a_" sqref="J44:J59 J2:J36 J38:J39">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMean" error="Something is wrong. Please enter a value between the minimum and maximum values" promptTitle="Mean" prompt="Enter the most likely value (or mean value) of the probability distribution. _x000a_" sqref="J38:J39 J2:J36 J44:J62">
       <formula1>H2</formula1>
       <formula2>I2</formula2>
     </dataValidation>
@@ -3563,13 +3667,13 @@
           <x14:formula1>
             <xm:f>ListItem!$B$3:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G59</xm:sqref>
+          <xm:sqref>G2:G62</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Distribution" prompt="Select a probability distribution">
           <x14:formula1>
             <xm:f>ListItem!$A$2:$A$16</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F59</xm:sqref>
+          <xm:sqref>F2:F62</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3601,7 +3705,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="2"/>
@@ -3668,7 +3772,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>

</xml_diff>

<commit_message>
No cross conta. in home prep. module
</commit_message>
<xml_diff>
--- a/data-input/estimated_variables.xlsx
+++ b/data-input/estimated_variables.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="180">
   <si>
     <t>Module</t>
   </si>
@@ -204,21 +204,6 @@
     <t>Exposure temperature during cooking in the “protected area”</t>
   </si>
   <si>
-    <t>P_h_wash</t>
-  </si>
-  <si>
-    <t>Probability of cross-contamination to occur (related to kitchen hygiene, represent the probability of not washing hands during chicken food preparation)</t>
-  </si>
-  <si>
-    <t>ml</t>
-  </si>
-  <si>
-    <t>V_ing</t>
-  </si>
-  <si>
-    <t>Volume of fluid ingested</t>
-  </si>
-  <si>
     <t xml:space="preserve">Count </t>
   </si>
   <si>
@@ -403,12 +388,6 @@
   </si>
   <si>
     <t>Prop_carc_yield</t>
-  </si>
-  <si>
-    <t>Prop_fluid</t>
-  </si>
-  <si>
-    <t>Proportion of cells in fluid</t>
   </si>
   <si>
     <t>assumption: chicken breast = quarter of whole carcass chicken</t>
@@ -595,12 +574,6 @@
   </si>
   <si>
     <t>F_freezer</t>
-  </si>
-  <si>
-    <t>V_dil_car</t>
-  </si>
-  <si>
-    <t>Volume of fluid diluting for a whole carcass</t>
   </si>
   <si>
     <t>D_value_alpha</t>
@@ -803,7 +776,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -822,8 +795,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -833,9 +804,7 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -847,7 +816,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1177,10 +1145,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P69"/>
+  <dimension ref="A1:P65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F10" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1203,7 +1171,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>1</v>
@@ -1218,7 +1186,7 @@
         <v>3</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="H1" s="8" t="s">
         <v>7</v>
@@ -1227,48 +1195,48 @@
         <v>8</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="M1" s="8" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="N1" s="8" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="O1" s="8" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="P1" s="8" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="32" t="s">
-        <v>100</v>
-      </c>
-      <c r="C2" s="36" t="s">
-        <v>101</v>
-      </c>
-      <c r="D2" s="37" t="s">
+      <c r="B2" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>97</v>
+      </c>
+      <c r="E2" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="E2" s="36" t="s">
-        <v>107</v>
-      </c>
       <c r="F2" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -1282,33 +1250,33 @@
       </c>
       <c r="N2" s="2"/>
       <c r="O2" s="3" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="P2" s="7" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="32" t="s">
-        <v>99</v>
-      </c>
-      <c r="C3" s="36" t="s">
-        <v>144</v>
-      </c>
-      <c r="D3" s="37" t="s">
-        <v>146</v>
-      </c>
-      <c r="E3" s="36" t="s">
-        <v>107</v>
+      <c r="B3" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>137</v>
+      </c>
+      <c r="D3" s="33" t="s">
+        <v>139</v>
+      </c>
+      <c r="E3" s="32" t="s">
+        <v>102</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
@@ -1319,8 +1287,8 @@
       </c>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
-      <c r="O3" s="35" t="s">
-        <v>142</v>
+      <c r="O3" s="31" t="s">
+        <v>135</v>
       </c>
       <c r="P3" s="4"/>
     </row>
@@ -1328,23 +1296,23 @@
       <c r="A4" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="32" t="s">
-        <v>99</v>
-      </c>
-      <c r="C4" s="36" t="s">
-        <v>145</v>
-      </c>
-      <c r="D4" s="37" t="s">
-        <v>147</v>
-      </c>
-      <c r="E4" s="36" t="s">
-        <v>107</v>
+      <c r="B4" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" s="32" t="s">
+        <v>138</v>
+      </c>
+      <c r="D4" s="33" t="s">
+        <v>140</v>
+      </c>
+      <c r="E4" s="32" t="s">
+        <v>102</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
@@ -1355,8 +1323,8 @@
       </c>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
-      <c r="O4" s="35" t="s">
-        <v>142</v>
+      <c r="O4" s="31" t="s">
+        <v>135</v>
       </c>
       <c r="P4" s="4"/>
     </row>
@@ -1364,23 +1332,23 @@
       <c r="A5" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="32" t="s">
+      <c r="B5" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>98</v>
+      </c>
+      <c r="D5" s="33" t="s">
         <v>99</v>
       </c>
-      <c r="C5" s="36" t="s">
-        <v>103</v>
-      </c>
-      <c r="D5" s="37" t="s">
-        <v>104</v>
-      </c>
-      <c r="E5" s="36" t="s">
-        <v>107</v>
+      <c r="E5" s="32" t="s">
+        <v>102</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H5" s="2">
         <v>0.157</v>
@@ -1395,34 +1363,34 @@
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
-      <c r="O5" s="35" t="s">
-        <v>142</v>
+      <c r="O5" s="31" t="s">
+        <v>135</v>
       </c>
       <c r="P5" s="4" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="32" t="s">
-        <v>99</v>
-      </c>
-      <c r="C6" s="36" t="s">
-        <v>105</v>
-      </c>
-      <c r="D6" s="37" t="s">
-        <v>106</v>
-      </c>
-      <c r="E6" s="36" t="s">
-        <v>82</v>
+      <c r="B6" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="C6" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="D6" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="E6" s="32" t="s">
+        <v>77</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H6" s="2">
         <v>18000000</v>
@@ -1438,33 +1406,33 @@
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" s="3" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="P6" s="4" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="32" t="s">
-        <v>99</v>
-      </c>
-      <c r="C7" s="36" t="s">
-        <v>126</v>
-      </c>
-      <c r="D7" s="37" t="s">
-        <v>134</v>
-      </c>
-      <c r="E7" s="36" t="s">
+      <c r="B7" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="C7" s="32" t="s">
+        <v>119</v>
+      </c>
+      <c r="D7" s="33" t="s">
+        <v>127</v>
+      </c>
+      <c r="E7" s="32" t="s">
         <v>23</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H7" s="2">
         <v>0</v>
@@ -1477,8 +1445,8 @@
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
-      <c r="O7" s="35" t="s">
-        <v>142</v>
+      <c r="O7" s="31" t="s">
+        <v>135</v>
       </c>
       <c r="P7" s="4"/>
     </row>
@@ -1486,23 +1454,23 @@
       <c r="A8" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="32" t="s">
-        <v>99</v>
-      </c>
-      <c r="C8" s="36" t="s">
-        <v>108</v>
-      </c>
-      <c r="D8" s="37" t="s">
-        <v>109</v>
-      </c>
-      <c r="E8" s="36" t="s">
-        <v>133</v>
+      <c r="B8" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>103</v>
+      </c>
+      <c r="D8" s="33" t="s">
+        <v>104</v>
+      </c>
+      <c r="E8" s="32" t="s">
+        <v>126</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
@@ -1513,32 +1481,32 @@
       </c>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
-      <c r="O8" s="35" t="s">
-        <v>142</v>
+      <c r="O8" s="31" t="s">
+        <v>135</v>
       </c>
       <c r="P8" s="4"/>
     </row>
     <row r="9" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="33" t="s">
+      <c r="A9" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="34" t="s">
-        <v>99</v>
-      </c>
-      <c r="C9" s="38" t="s">
-        <v>112</v>
-      </c>
-      <c r="D9" s="39" t="s">
-        <v>110</v>
-      </c>
-      <c r="E9" s="38" t="s">
+      <c r="B9" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="C9" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="D9" s="35" t="s">
+        <v>105</v>
+      </c>
+      <c r="E9" s="34" t="s">
         <v>32</v>
       </c>
       <c r="F9" s="9" t="s">
         <v>5</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H9" s="9">
         <v>4.4000000000000004</v>
@@ -1554,33 +1522,33 @@
       <c r="M9" s="9"/>
       <c r="N9" s="9"/>
       <c r="O9" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="P9" s="46" t="s">
-        <v>150</v>
+        <v>153</v>
+      </c>
+      <c r="P9" s="41" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="C10" s="40" t="s">
-        <v>119</v>
-      </c>
-      <c r="D10" s="37" t="s">
+      <c r="B10" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" s="36" t="s">
+        <v>114</v>
+      </c>
+      <c r="D10" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="36" t="s">
+      <c r="E10" s="32" t="s">
         <v>12</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>5</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H10" s="2">
         <v>1</v>
@@ -1596,7 +1564,7 @@
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
       <c r="O10" s="2" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="P10" s="2"/>
     </row>
@@ -1604,23 +1572,23 @@
       <c r="A11" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="C11" s="36" t="s">
+      <c r="B11" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="37" t="s">
+      <c r="D11" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="36" t="s">
+      <c r="E11" s="32" t="s">
         <v>15</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>6</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H11" s="2">
         <v>0</v>
@@ -1634,7 +1602,7 @@
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
       <c r="O11" s="2" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="P11" s="2"/>
     </row>
@@ -1642,23 +1610,23 @@
       <c r="A12" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="C12" s="41" t="s">
+      <c r="B12" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="42" t="s">
+      <c r="D12" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="41" t="s">
-        <v>61</v>
+      <c r="E12" s="37" t="s">
+        <v>56</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>4</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H12" s="5">
         <v>1.5</v>
@@ -1674,7 +1642,7 @@
       <c r="M12" s="5"/>
       <c r="N12" s="5"/>
       <c r="O12" s="5" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="P12" s="5"/>
     </row>
@@ -1682,23 +1650,23 @@
       <c r="A13" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="21" t="s">
-        <v>99</v>
-      </c>
-      <c r="C13" s="44" t="s">
-        <v>148</v>
-      </c>
-      <c r="D13" s="37" t="s">
-        <v>151</v>
-      </c>
-      <c r="E13" s="36" t="s">
-        <v>131</v>
+      <c r="B13" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="C13" s="39" t="s">
+        <v>141</v>
+      </c>
+      <c r="D13" s="33" t="s">
+        <v>144</v>
+      </c>
+      <c r="E13" s="32" t="s">
+        <v>124</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
@@ -1710,7 +1678,7 @@
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
       <c r="O13" s="2" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="P13" s="2"/>
     </row>
@@ -1718,23 +1686,23 @@
       <c r="A14" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="21" t="s">
-        <v>99</v>
-      </c>
-      <c r="C14" s="44" t="s">
-        <v>149</v>
-      </c>
-      <c r="D14" s="37" t="s">
-        <v>152</v>
-      </c>
-      <c r="E14" s="36" t="s">
-        <v>131</v>
+      <c r="B14" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="C14" s="39" t="s">
+        <v>142</v>
+      </c>
+      <c r="D14" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="E14" s="32" t="s">
+        <v>124</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
@@ -1746,7 +1714,7 @@
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
       <c r="O14" s="2" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="P14" s="2"/>
     </row>
@@ -1754,23 +1722,23 @@
       <c r="A15" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="21" t="s">
-        <v>99</v>
-      </c>
-      <c r="C15" s="44" t="s">
-        <v>136</v>
-      </c>
-      <c r="D15" s="45" t="s">
-        <v>137</v>
-      </c>
-      <c r="E15" s="36" t="s">
-        <v>131</v>
+      <c r="B15" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="C15" s="39" t="s">
+        <v>129</v>
+      </c>
+      <c r="D15" s="40" t="s">
+        <v>130</v>
+      </c>
+      <c r="E15" s="32" t="s">
+        <v>124</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
@@ -1784,33 +1752,33 @@
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
       <c r="O15" s="3" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="21" t="s">
-        <v>99</v>
-      </c>
-      <c r="C16" s="36" t="s">
-        <v>155</v>
-      </c>
-      <c r="D16" s="37" t="s">
-        <v>157</v>
-      </c>
-      <c r="E16" s="36" t="s">
+      <c r="B16" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="C16" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="D16" s="33" t="s">
+        <v>150</v>
+      </c>
+      <c r="E16" s="32" t="s">
         <v>10</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
@@ -1822,7 +1790,7 @@
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
       <c r="O16" s="3" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="P16" s="2"/>
     </row>
@@ -1830,23 +1798,23 @@
       <c r="A17" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="21" t="s">
-        <v>99</v>
-      </c>
-      <c r="C17" s="36" t="s">
-        <v>156</v>
-      </c>
-      <c r="D17" s="37" t="s">
-        <v>158</v>
-      </c>
-      <c r="E17" s="36" t="s">
+      <c r="B17" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="C17" s="32" t="s">
+        <v>149</v>
+      </c>
+      <c r="D17" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="E17" s="32" t="s">
         <v>10</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
@@ -1858,7 +1826,7 @@
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
       <c r="O17" s="3" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="P17" s="2"/>
     </row>
@@ -1866,23 +1834,23 @@
       <c r="A18" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="21" t="s">
-        <v>99</v>
-      </c>
-      <c r="C18" s="36" t="s">
-        <v>127</v>
-      </c>
-      <c r="D18" s="37" t="s">
+      <c r="B18" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="C18" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="D18" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="E18" s="36" t="s">
-        <v>159</v>
+      <c r="E18" s="32" t="s">
+        <v>152</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>5</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H18" s="3">
         <v>-4.01</v>
@@ -1898,33 +1866,33 @@
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
       <c r="O18" s="3" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="21" t="s">
-        <v>99</v>
-      </c>
-      <c r="C19" s="36" t="s">
+      <c r="B19" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="C19" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="D19" s="37" t="s">
+      <c r="D19" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="E19" s="36" t="s">
+      <c r="E19" s="32" t="s">
         <v>23</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
@@ -1936,7 +1904,7 @@
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
       <c r="O19" s="3" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="P19" s="2"/>
     </row>
@@ -1944,23 +1912,23 @@
       <c r="A20" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="21" t="s">
-        <v>99</v>
-      </c>
-      <c r="C20" s="36" t="s">
+      <c r="B20" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="C20" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="D20" s="37" t="s">
-        <v>138</v>
-      </c>
-      <c r="E20" s="36" t="s">
+      <c r="D20" s="33" t="s">
+        <v>131</v>
+      </c>
+      <c r="E20" s="32" t="s">
         <v>23</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="H20" s="2">
         <v>0</v>
@@ -1978,7 +1946,7 @@
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
       <c r="O20" s="3" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="P20" s="3"/>
     </row>
@@ -1986,23 +1954,23 @@
       <c r="A21" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="21" t="s">
-        <v>99</v>
-      </c>
-      <c r="C21" s="36" t="s">
-        <v>80</v>
-      </c>
-      <c r="D21" s="37" t="s">
-        <v>81</v>
-      </c>
-      <c r="E21" s="36" t="s">
-        <v>82</v>
+      <c r="B21" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="C21" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="D21" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="E21" s="32" t="s">
+        <v>77</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>5</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H21" s="2">
         <v>0.54</v>
@@ -2018,30 +1986,30 @@
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
       <c r="O21" s="3" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A22" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="21" t="s">
-        <v>99</v>
-      </c>
-      <c r="C22" s="36" t="s">
+      <c r="B22" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="C22" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="D22" s="37" t="s">
+      <c r="D22" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="E22" s="36" t="s">
+      <c r="E22" s="32" t="s">
         <v>23</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>5</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H22" s="2">
         <v>0.03</v>
@@ -2057,7 +2025,7 @@
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
       <c r="O22" s="3" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="P22" s="2"/>
     </row>
@@ -2065,23 +2033,23 @@
       <c r="A23" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="21" t="s">
-        <v>99</v>
-      </c>
-      <c r="C23" s="36" t="s">
+      <c r="B23" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="C23" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="D23" s="37" t="s">
-        <v>116</v>
-      </c>
-      <c r="E23" s="36" t="s">
+      <c r="D23" s="33" t="s">
+        <v>111</v>
+      </c>
+      <c r="E23" s="32" t="s">
         <v>34</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>5</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H23" s="3">
         <v>0.06</v>
@@ -2097,33 +2065,33 @@
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
       <c r="O23" s="3" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="P23" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A24" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B24" s="21" t="s">
-        <v>99</v>
-      </c>
-      <c r="C24" s="36" t="s">
-        <v>165</v>
-      </c>
-      <c r="D24" s="37" t="s">
-        <v>167</v>
-      </c>
-      <c r="E24" s="36" t="s">
+      <c r="B24" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="C24" s="32" t="s">
+        <v>158</v>
+      </c>
+      <c r="D24" s="33" t="s">
+        <v>160</v>
+      </c>
+      <c r="E24" s="32" t="s">
         <v>10</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>6</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H24" s="3">
         <v>0</v>
@@ -2137,7 +2105,7 @@
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
       <c r="O24" s="3" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="P24" s="7"/>
     </row>
@@ -2145,23 +2113,23 @@
       <c r="A25" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="21" t="s">
-        <v>99</v>
-      </c>
-      <c r="C25" s="36" t="s">
-        <v>161</v>
-      </c>
-      <c r="D25" s="37" t="s">
-        <v>162</v>
-      </c>
-      <c r="E25" s="36" t="s">
-        <v>159</v>
+      <c r="B25" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="C25" s="32" t="s">
+        <v>154</v>
+      </c>
+      <c r="D25" s="33" t="s">
+        <v>155</v>
+      </c>
+      <c r="E25" s="32" t="s">
+        <v>152</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>5</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H25" s="2">
         <v>-1.29</v>
@@ -2176,34 +2144,34 @@
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
-      <c r="O25" s="35" t="s">
-        <v>142</v>
+      <c r="O25" s="31" t="s">
+        <v>135</v>
       </c>
       <c r="P25" s="2" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A26" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B26" s="21" t="s">
-        <v>99</v>
-      </c>
-      <c r="C26" s="36" t="s">
-        <v>164</v>
-      </c>
-      <c r="D26" s="37" t="s">
-        <v>163</v>
-      </c>
-      <c r="E26" s="36" t="s">
-        <v>159</v>
+      <c r="B26" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="C26" s="32" t="s">
+        <v>157</v>
+      </c>
+      <c r="D26" s="33" t="s">
+        <v>156</v>
+      </c>
+      <c r="E26" s="32" t="s">
+        <v>152</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>5</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H26" s="2">
         <v>-1.28</v>
@@ -2218,34 +2186,34 @@
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
-      <c r="O26" s="35" t="s">
-        <v>142</v>
+      <c r="O26" s="31" t="s">
+        <v>135</v>
       </c>
       <c r="P26" s="2" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A27" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B27" s="21" t="s">
-        <v>99</v>
-      </c>
-      <c r="C27" s="36" t="s">
-        <v>128</v>
-      </c>
-      <c r="D27" s="37" t="s">
+      <c r="B27" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="C27" s="32" t="s">
+        <v>121</v>
+      </c>
+      <c r="D27" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="E27" s="36" t="s">
+      <c r="E27" s="32" t="s">
         <v>10</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>6</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H27" s="2">
         <v>0</v>
@@ -2258,8 +2226,8 @@
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
-      <c r="O27" s="35" t="s">
-        <v>142</v>
+      <c r="O27" s="31" t="s">
+        <v>135</v>
       </c>
       <c r="P27" s="2"/>
     </row>
@@ -2267,23 +2235,23 @@
       <c r="A28" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B28" s="21" t="s">
-        <v>99</v>
-      </c>
-      <c r="C28" s="36" t="s">
-        <v>129</v>
-      </c>
-      <c r="D28" s="37" t="s">
-        <v>168</v>
-      </c>
-      <c r="E28" s="36" t="s">
+      <c r="B28" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="C28" s="32" t="s">
+        <v>122</v>
+      </c>
+      <c r="D28" s="33" t="s">
+        <v>161</v>
+      </c>
+      <c r="E28" s="32" t="s">
         <v>34</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>4</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H28" s="3">
         <v>5.1050499999999999E-2</v>
@@ -2298,8 +2266,8 @@
       <c r="L28" s="2"/>
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
-      <c r="O28" s="35" t="s">
-        <v>142</v>
+      <c r="O28" s="31" t="s">
+        <v>135</v>
       </c>
       <c r="P28" s="2"/>
     </row>
@@ -2307,23 +2275,23 @@
       <c r="A29" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B29" s="21" t="s">
-        <v>99</v>
-      </c>
-      <c r="C29" s="36" t="s">
-        <v>113</v>
-      </c>
-      <c r="D29" s="37" t="s">
-        <v>85</v>
-      </c>
-      <c r="E29" s="36" t="s">
+      <c r="B29" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="C29" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="D29" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="E29" s="32" t="s">
         <v>10</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>4</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H29" s="3">
         <v>0.01</v>
@@ -2340,8 +2308,8 @@
       </c>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
-      <c r="O29" s="35" t="s">
-        <v>142</v>
+      <c r="O29" s="31" t="s">
+        <v>135</v>
       </c>
       <c r="P29" s="2"/>
     </row>
@@ -2349,23 +2317,23 @@
       <c r="A30" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B30" s="22" t="s">
-        <v>99</v>
-      </c>
-      <c r="C30" s="38" t="s">
-        <v>83</v>
-      </c>
-      <c r="D30" s="39" t="s">
-        <v>84</v>
-      </c>
-      <c r="E30" s="38" t="s">
+      <c r="B30" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="C30" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="D30" s="35" t="s">
+        <v>79</v>
+      </c>
+      <c r="E30" s="34" t="s">
         <v>23</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H30" s="9"/>
       <c r="I30" s="9"/>
@@ -2378,8 +2346,8 @@
         <v>3.15</v>
       </c>
       <c r="N30" s="9"/>
-      <c r="O30" s="51" t="s">
-        <v>142</v>
+      <c r="O30" s="46" t="s">
+        <v>135</v>
       </c>
       <c r="P30" s="9"/>
     </row>
@@ -2387,23 +2355,23 @@
       <c r="A31" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="C31" s="36" t="s">
+      <c r="B31" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C31" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="D31" s="37" t="s">
+      <c r="D31" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="E31" s="36" t="s">
+      <c r="E31" s="32" t="s">
         <v>23</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>5</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H31" s="2">
         <v>0.14000000000000001</v>
@@ -2418,8 +2386,8 @@
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
-      <c r="O31" s="35" t="s">
-        <v>142</v>
+      <c r="O31" s="31" t="s">
+        <v>135</v>
       </c>
       <c r="P31" s="2"/>
     </row>
@@ -2427,23 +2395,23 @@
       <c r="A32" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B32" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="C32" s="36" t="s">
+      <c r="B32" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C32" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="D32" s="37" t="s">
+      <c r="D32" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="E32" s="36" t="s">
+      <c r="E32" s="32" t="s">
         <v>12</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>6</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H32" s="3">
         <v>1</v>
@@ -2457,64 +2425,64 @@
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
       <c r="O32" s="3" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="P32" s="2"/>
     </row>
     <row r="33" spans="1:16" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="47" t="s">
+      <c r="A33" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="B33" s="48" t="s">
-        <v>65</v>
-      </c>
-      <c r="C33" s="49" t="s">
-        <v>120</v>
-      </c>
-      <c r="D33" s="50" t="s">
-        <v>117</v>
-      </c>
-      <c r="E33" s="49" t="s">
+      <c r="B33" s="43" t="s">
+        <v>60</v>
+      </c>
+      <c r="C33" s="44" t="s">
+        <v>115</v>
+      </c>
+      <c r="D33" s="45" t="s">
+        <v>112</v>
+      </c>
+      <c r="E33" s="44" t="s">
         <v>34</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="J33" s="6"/>
       <c r="L33" s="5">
         <v>0.25</v>
       </c>
       <c r="O33" s="6" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="P33" s="5" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A34" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B34" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="C34" s="36" t="s">
-        <v>87</v>
-      </c>
-      <c r="D34" s="37" t="s">
-        <v>88</v>
-      </c>
-      <c r="E34" s="36" t="s">
+      <c r="B34" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="C34" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="D34" s="33" t="s">
+        <v>83</v>
+      </c>
+      <c r="E34" s="32" t="s">
         <v>42</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
@@ -2526,7 +2494,7 @@
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
       <c r="O34" s="3" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="P34" s="2"/>
     </row>
@@ -2534,23 +2502,23 @@
       <c r="A35" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B35" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="C35" s="36" t="s">
-        <v>89</v>
-      </c>
-      <c r="D35" s="37" t="s">
-        <v>90</v>
-      </c>
-      <c r="E35" s="36" t="s">
+      <c r="B35" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="C35" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="D35" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="E35" s="32" t="s">
         <v>42</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>4</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H35" s="2">
         <v>35</v>
@@ -2566,7 +2534,7 @@
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
       <c r="O35" s="3" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="P35" s="2"/>
     </row>
@@ -2574,23 +2542,23 @@
       <c r="A36" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B36" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="C36" s="36" t="s">
-        <v>130</v>
-      </c>
-      <c r="D36" s="37" t="s">
-        <v>91</v>
-      </c>
-      <c r="E36" s="36" t="s">
+      <c r="B36" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="C36" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="D36" s="33" t="s">
         <v>86</v>
+      </c>
+      <c r="E36" s="32" t="s">
+        <v>81</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>5</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H36" s="2">
         <v>-0.3</v>
@@ -2606,7 +2574,7 @@
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
       <c r="O36" s="3" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="P36" s="2"/>
     </row>
@@ -2614,23 +2582,23 @@
       <c r="A37" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B37" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="C37" s="36" t="s">
-        <v>182</v>
-      </c>
-      <c r="D37" s="37" t="s">
-        <v>181</v>
-      </c>
-      <c r="E37" s="36" t="s">
+      <c r="B37" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="C37" s="32" t="s">
+        <v>175</v>
+      </c>
+      <c r="D37" s="33" t="s">
+        <v>174</v>
+      </c>
+      <c r="E37" s="32" t="s">
         <v>34</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
@@ -2641,7 +2609,7 @@
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
       <c r="O37" s="3" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="P37" s="2"/>
     </row>
@@ -2649,23 +2617,23 @@
       <c r="A38" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B38" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="C38" s="36" t="s">
-        <v>92</v>
-      </c>
-      <c r="D38" s="37" t="s">
-        <v>93</v>
-      </c>
-      <c r="E38" s="36" t="s">
+      <c r="B38" s="25" t="s">
         <v>94</v>
       </c>
+      <c r="C38" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="D38" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="E38" s="32" t="s">
+        <v>89</v>
+      </c>
       <c r="F38" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
@@ -2677,7 +2645,7 @@
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
       <c r="O38" s="3" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="P38" s="2"/>
     </row>
@@ -2685,23 +2653,23 @@
       <c r="A39" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B39" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="C39" s="38" t="s">
-        <v>121</v>
-      </c>
-      <c r="D39" s="39" t="s">
-        <v>95</v>
-      </c>
-      <c r="E39" s="38" t="s">
-        <v>82</v>
+      <c r="B39" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="C39" s="34" t="s">
+        <v>116</v>
+      </c>
+      <c r="D39" s="35" t="s">
+        <v>90</v>
+      </c>
+      <c r="E39" s="34" t="s">
+        <v>77</v>
       </c>
       <c r="F39" s="9" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G39" s="9" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H39" s="9"/>
       <c r="I39" s="9"/>
@@ -2713,7 +2681,7 @@
       <c r="M39" s="9"/>
       <c r="N39" s="9"/>
       <c r="O39" s="10" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="P39" s="9"/>
     </row>
@@ -2721,23 +2689,23 @@
       <c r="A40" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B40" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="C40" s="36" t="s">
-        <v>169</v>
-      </c>
-      <c r="D40" s="37" t="s">
-        <v>118</v>
-      </c>
-      <c r="E40" s="36" t="s">
+      <c r="B40" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="C40" s="32" t="s">
+        <v>162</v>
+      </c>
+      <c r="D40" s="33" t="s">
+        <v>113</v>
+      </c>
+      <c r="E40" s="32" t="s">
         <v>12</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>
@@ -2748,7 +2716,7 @@
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
       <c r="O40" s="3" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="P40" s="2"/>
     </row>
@@ -2756,23 +2724,23 @@
       <c r="A41" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B41" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="C41" s="36" t="s">
-        <v>170</v>
-      </c>
-      <c r="D41" s="37" t="s">
-        <v>173</v>
-      </c>
-      <c r="E41" s="36" t="s">
+      <c r="B41" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="C41" s="32" t="s">
+        <v>163</v>
+      </c>
+      <c r="D41" s="33" t="s">
+        <v>166</v>
+      </c>
+      <c r="E41" s="32" t="s">
         <v>12</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
@@ -2783,7 +2751,7 @@
       <c r="M41" s="2"/>
       <c r="N41" s="2"/>
       <c r="O41" s="3" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="P41" s="2"/>
     </row>
@@ -2791,23 +2759,23 @@
       <c r="A42" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B42" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="C42" s="36" t="s">
-        <v>171</v>
-      </c>
-      <c r="D42" s="37" t="s">
-        <v>174</v>
-      </c>
-      <c r="E42" s="36" t="s">
+      <c r="B42" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="C42" s="32" t="s">
+        <v>164</v>
+      </c>
+      <c r="D42" s="33" t="s">
+        <v>167</v>
+      </c>
+      <c r="E42" s="32" t="s">
         <v>12</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
@@ -2818,7 +2786,7 @@
       <c r="M42" s="2"/>
       <c r="N42" s="2"/>
       <c r="O42" s="3" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="P42" s="2"/>
     </row>
@@ -2826,23 +2794,23 @@
       <c r="A43" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B43" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="C43" s="36" t="s">
-        <v>172</v>
-      </c>
-      <c r="D43" s="37" t="s">
-        <v>175</v>
-      </c>
-      <c r="E43" s="36" t="s">
+      <c r="B43" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="C43" s="32" t="s">
+        <v>165</v>
+      </c>
+      <c r="D43" s="33" t="s">
+        <v>168</v>
+      </c>
+      <c r="E43" s="32" t="s">
         <v>12</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
@@ -2853,7 +2821,7 @@
       <c r="M43" s="2"/>
       <c r="N43" s="2"/>
       <c r="O43" s="3" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="P43" s="2"/>
     </row>
@@ -2861,23 +2829,23 @@
       <c r="A44" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B44" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="C44" s="36" t="s">
-        <v>122</v>
-      </c>
-      <c r="D44" s="37" t="s">
+      <c r="B44" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="C44" s="32" t="s">
+        <v>117</v>
+      </c>
+      <c r="D44" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="E44" s="36" t="s">
+      <c r="E44" s="32" t="s">
         <v>34</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>6</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H44" s="2">
         <v>0.6</v>
@@ -2891,7 +2859,7 @@
       <c r="M44" s="2"/>
       <c r="N44" s="2"/>
       <c r="O44" s="3" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="P44" s="2"/>
     </row>
@@ -2899,23 +2867,23 @@
       <c r="A45" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B45" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="C45" s="36" t="s">
+      <c r="B45" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="C45" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="D45" s="37" t="s">
+      <c r="D45" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="E45" s="36" t="s">
+      <c r="E45" s="32" t="s">
         <v>39</v>
       </c>
       <c r="F45" s="2" t="s">
         <v>5</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H45" s="2">
         <v>1</v>
@@ -2931,7 +2899,7 @@
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
       <c r="O45" s="3" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="P45" s="2"/>
     </row>
@@ -2939,23 +2907,23 @@
       <c r="A46" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B46" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="C46" s="36" t="s">
+      <c r="B46" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="C46" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="D46" s="37" t="s">
-        <v>139</v>
-      </c>
-      <c r="E46" s="36" t="s">
+      <c r="D46" s="33" t="s">
+        <v>132</v>
+      </c>
+      <c r="E46" s="32" t="s">
         <v>44</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H46" s="2"/>
       <c r="I46" s="2"/>
@@ -2969,7 +2937,7 @@
       <c r="M46" s="2"/>
       <c r="N46" s="2"/>
       <c r="O46" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="P46" s="2"/>
     </row>
@@ -2977,23 +2945,23 @@
       <c r="A47" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B47" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="C47" s="36" t="s">
+      <c r="B47" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="C47" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="D47" s="37" t="s">
-        <v>140</v>
-      </c>
-      <c r="E47" s="36" t="s">
+      <c r="D47" s="33" t="s">
+        <v>133</v>
+      </c>
+      <c r="E47" s="32" t="s">
         <v>39</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>
@@ -3007,7 +2975,7 @@
       <c r="M47" s="2"/>
       <c r="N47" s="2"/>
       <c r="O47" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="P47" s="2"/>
     </row>
@@ -3015,23 +2983,23 @@
       <c r="A48" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B48" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="C48" s="36" t="s">
+      <c r="B48" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="C48" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="D48" s="37" t="s">
+      <c r="D48" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="E48" s="36" t="s">
+      <c r="E48" s="32" t="s">
         <v>42</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="H48" s="2">
         <v>-6.67</v>
@@ -3049,7 +3017,7 @@
       <c r="M48" s="2"/>
       <c r="N48" s="2"/>
       <c r="O48" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="P48" s="2"/>
     </row>
@@ -3057,23 +3025,23 @@
       <c r="A49" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B49" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="C49" s="36" t="s">
+      <c r="B49" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="C49" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="D49" s="37" t="s">
+      <c r="D49" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="E49" s="36" t="s">
+      <c r="E49" s="32" t="s">
         <v>42</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="H49" s="3">
         <v>-5.56</v>
@@ -3093,7 +3061,7 @@
         <v>-22.914999999999999</v>
       </c>
       <c r="O49" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="P49" s="2"/>
     </row>
@@ -3101,23 +3069,23 @@
       <c r="A50" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B50" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="C50" s="52" t="s">
+      <c r="B50" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="C50" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="D50" s="53" t="s">
+      <c r="D50" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="E50" s="52" t="s">
+      <c r="E50" s="47" t="s">
         <v>42</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="H50" s="2">
         <v>-4.4400000000000004</v>
@@ -3135,7 +3103,7 @@
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
       <c r="O50" s="3" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="P50" s="2"/>
     </row>
@@ -3143,23 +3111,23 @@
       <c r="A51" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B51" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="C51" s="52" t="s">
-        <v>177</v>
-      </c>
-      <c r="D51" s="53" t="s">
-        <v>178</v>
-      </c>
-      <c r="E51" s="36" t="s">
+      <c r="B51" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="C51" s="47" t="s">
+        <v>170</v>
+      </c>
+      <c r="D51" s="48" t="s">
+        <v>171</v>
+      </c>
+      <c r="E51" s="32" t="s">
         <v>34</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H51" s="2"/>
       <c r="I51" s="2"/>
@@ -3171,7 +3139,7 @@
       <c r="M51" s="2"/>
       <c r="N51" s="2"/>
       <c r="O51" s="2" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="P51" s="2"/>
     </row>
@@ -3179,23 +3147,23 @@
       <c r="A52" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="B52" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="C52" s="41" t="s">
-        <v>179</v>
-      </c>
-      <c r="D52" s="42" t="s">
-        <v>180</v>
-      </c>
-      <c r="E52" s="49" t="s">
+      <c r="B52" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="C52" s="37" t="s">
+        <v>172</v>
+      </c>
+      <c r="D52" s="38" t="s">
+        <v>173</v>
+      </c>
+      <c r="E52" s="44" t="s">
         <v>34</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H52" s="5"/>
       <c r="I52" s="5"/>
@@ -3207,7 +3175,7 @@
       <c r="M52" s="5"/>
       <c r="N52" s="5"/>
       <c r="O52" s="5" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="P52" s="5"/>
     </row>
@@ -3215,23 +3183,23 @@
       <c r="A53" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="B53" s="28" t="s">
-        <v>99</v>
-      </c>
-      <c r="C53" s="36" t="s">
-        <v>96</v>
-      </c>
-      <c r="D53" s="37" t="s">
-        <v>97</v>
-      </c>
-      <c r="E53" s="36" t="s">
+      <c r="B53" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="C53" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="D53" s="33" t="s">
+        <v>92</v>
+      </c>
+      <c r="E53" s="32" t="s">
         <v>34</v>
       </c>
       <c r="F53" s="2" t="s">
         <v>4</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H53" s="2">
         <v>0.1</v>
@@ -3247,83 +3215,81 @@
       <c r="M53" s="2"/>
       <c r="N53" s="2"/>
       <c r="O53" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="P53" s="2"/>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A54" s="18" t="s">
+      <c r="A54" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="B54" s="29" t="s">
-        <v>99</v>
-      </c>
-      <c r="C54" s="38" t="s">
-        <v>123</v>
-      </c>
-      <c r="D54" s="39" t="s">
-        <v>124</v>
-      </c>
-      <c r="E54" s="43" t="s">
-        <v>34</v>
-      </c>
-      <c r="F54" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="G54" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="H54" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="I54" s="10">
-        <v>0.1</v>
-      </c>
-      <c r="J54" s="9"/>
-      <c r="K54" s="9"/>
-      <c r="L54" s="9"/>
-      <c r="M54" s="9"/>
-      <c r="N54" s="9"/>
+      <c r="B54" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="C54" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="D54" s="33" t="s">
+        <v>134</v>
+      </c>
+      <c r="E54" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H54" s="2"/>
+      <c r="I54" s="2"/>
+      <c r="J54" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="K54" s="2">
+        <v>2.1199999999999999E-3</v>
+      </c>
+      <c r="L54" s="2"/>
+      <c r="M54" s="2"/>
+      <c r="N54" s="2"/>
       <c r="O54" t="s">
-        <v>142</v>
-      </c>
-      <c r="P54" s="9"/>
+        <v>135</v>
+      </c>
+      <c r="P54" s="2"/>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A55" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="B55" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="C55" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="D55" s="37" t="s">
-        <v>141</v>
-      </c>
-      <c r="E55" s="36" t="s">
-        <v>23</v>
+      <c r="B55" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="C55" s="32" t="s">
+        <v>176</v>
+      </c>
+      <c r="D55" s="33" t="s">
+        <v>177</v>
+      </c>
+      <c r="E55" s="32" t="s">
+        <v>10</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H55" s="2"/>
       <c r="I55" s="2"/>
-      <c r="J55" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="K55" s="2">
-        <v>2.1199999999999999E-3</v>
-      </c>
-      <c r="L55" s="2"/>
+      <c r="J55" s="3"/>
+      <c r="K55" s="2"/>
+      <c r="L55" s="2">
+        <v>8.58</v>
+      </c>
       <c r="M55" s="2"/>
       <c r="N55" s="2"/>
       <c r="O55" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="P55" s="2"/>
     </row>
@@ -3331,37 +3297,35 @@
       <c r="A56" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="B56" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="C56" s="36" t="s">
-        <v>183</v>
-      </c>
-      <c r="D56" s="37" t="s">
-        <v>184</v>
-      </c>
-      <c r="E56" s="36" t="s">
+      <c r="B56" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="C56" s="32" t="s">
+        <v>178</v>
+      </c>
+      <c r="D56" s="33" t="s">
+        <v>179</v>
+      </c>
+      <c r="E56" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="F56" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F56" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="G56" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="H56" s="2">
-        <v>150</v>
-      </c>
-      <c r="I56" s="2">
-        <v>250</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="H56" s="2"/>
+      <c r="I56" s="2"/>
       <c r="J56" s="3"/>
       <c r="K56" s="2"/>
-      <c r="L56" s="2"/>
+      <c r="L56" s="2">
+        <v>-0.13900000000000001</v>
+      </c>
       <c r="M56" s="2"/>
       <c r="N56" s="2"/>
       <c r="O56" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="P56" s="2"/>
     </row>
@@ -3369,35 +3333,39 @@
       <c r="A57" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="B57" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="C57" s="36" t="s">
-        <v>185</v>
-      </c>
-      <c r="D57" s="37" t="s">
-        <v>186</v>
-      </c>
-      <c r="E57" s="36" t="s">
-        <v>10</v>
+      <c r="B57" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="C57" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="D57" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="E57" s="32" t="s">
+        <v>44</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>63</v>
+        <v>4</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="H57" s="2"/>
-      <c r="I57" s="2"/>
-      <c r="J57" s="3"/>
+        <v>73</v>
+      </c>
+      <c r="H57" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="I57" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="J57" s="3">
+        <v>1</v>
+      </c>
       <c r="K57" s="2"/>
-      <c r="L57" s="2">
-        <v>8.58</v>
-      </c>
+      <c r="L57" s="2"/>
       <c r="M57" s="2"/>
       <c r="N57" s="2"/>
       <c r="O57" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="P57" s="2"/>
     </row>
@@ -3405,230 +3373,78 @@
       <c r="A58" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="B58" s="30" t="s">
+      <c r="B58" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="C58" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="D58" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="E58" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G58" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H58" s="2">
+        <v>60</v>
+      </c>
+      <c r="I58" s="2">
         <v>65</v>
       </c>
-      <c r="C58" s="36" t="s">
-        <v>187</v>
-      </c>
-      <c r="D58" s="37" t="s">
-        <v>188</v>
-      </c>
-      <c r="E58" s="36" t="s">
-        <v>10</v>
-      </c>
-      <c r="F58" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="G58" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="H58" s="2"/>
-      <c r="I58" s="2"/>
-      <c r="J58" s="3"/>
+      <c r="J58" s="3">
+        <v>64</v>
+      </c>
       <c r="K58" s="2"/>
-      <c r="L58" s="2">
-        <v>-0.13900000000000001</v>
-      </c>
+      <c r="L58" s="2"/>
       <c r="M58" s="2"/>
       <c r="N58" s="2"/>
       <c r="O58" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="P58" s="2"/>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A59" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="B59" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="C59" s="36" t="s">
-        <v>52</v>
-      </c>
-      <c r="D59" s="37" t="s">
-        <v>53</v>
-      </c>
-      <c r="E59" s="36" t="s">
-        <v>44</v>
-      </c>
-      <c r="F59" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G59" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="H59" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="I59" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="J59" s="3">
-        <v>1</v>
-      </c>
-      <c r="K59" s="2"/>
       <c r="L59" s="2"/>
       <c r="M59" s="2"/>
       <c r="N59" s="2"/>
-      <c r="O59" t="s">
-        <v>142</v>
-      </c>
-      <c r="P59" s="2"/>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A60" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="B60" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="C60" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="D60" s="37" t="s">
-        <v>55</v>
-      </c>
-      <c r="E60" s="36" t="s">
-        <v>42</v>
-      </c>
-      <c r="F60" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G60" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="H60" s="2">
-        <v>60</v>
-      </c>
-      <c r="I60" s="2">
-        <v>65</v>
-      </c>
-      <c r="J60" s="3">
-        <v>64</v>
-      </c>
       <c r="K60" s="2"/>
-      <c r="L60" s="2"/>
-      <c r="M60" s="2"/>
-      <c r="N60" s="2"/>
-      <c r="O60" t="s">
-        <v>142</v>
-      </c>
-      <c r="P60" s="2"/>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A61" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="B61" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="C61" s="36" t="s">
-        <v>56</v>
-      </c>
-      <c r="D61" s="37" t="s">
-        <v>57</v>
-      </c>
-      <c r="E61" s="36" t="s">
-        <v>23</v>
-      </c>
-      <c r="F61" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G61" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="H61" s="3">
-        <v>0.38</v>
-      </c>
-      <c r="I61" s="2">
-        <v>1</v>
-      </c>
-      <c r="J61" s="2"/>
       <c r="K61" s="2"/>
-      <c r="L61" s="2"/>
-      <c r="M61" s="2"/>
-      <c r="N61" s="2"/>
-      <c r="O61" t="s">
-        <v>142</v>
-      </c>
-      <c r="P61" s="2"/>
-    </row>
-    <row r="62" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A62" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="B62" s="31" t="s">
-        <v>65</v>
-      </c>
-      <c r="C62" s="41" t="s">
-        <v>59</v>
-      </c>
-      <c r="D62" s="42" t="s">
-        <v>60</v>
-      </c>
-      <c r="E62" s="41" t="s">
-        <v>58</v>
-      </c>
-      <c r="F62" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G62" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="H62" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="I62" s="5">
-        <v>1.5</v>
-      </c>
-      <c r="J62" s="5"/>
-      <c r="K62" s="5"/>
-      <c r="L62" s="5"/>
-      <c r="M62" s="5"/>
-      <c r="N62" s="5"/>
-      <c r="O62" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="P62" s="5"/>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="K62" s="2"/>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="L63" s="2"/>
-      <c r="M63" s="2"/>
-      <c r="N63" s="2"/>
+      <c r="K63" s="2"/>
+      <c r="O63" s="2"/>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.35">
       <c r="K64" s="2"/>
-    </row>
-    <row r="65" spans="11:15" x14ac:dyDescent="0.35">
-      <c r="K65" s="2"/>
-    </row>
-    <row r="66" spans="11:15" x14ac:dyDescent="0.35">
-      <c r="K66" s="2"/>
-    </row>
-    <row r="67" spans="11:15" x14ac:dyDescent="0.35">
-      <c r="K67" s="2"/>
-      <c r="O67" s="2"/>
-    </row>
-    <row r="68" spans="11:15" x14ac:dyDescent="0.35">
-      <c r="K68" s="2"/>
-      <c r="O68" s="2"/>
-    </row>
-    <row r="69" spans="11:15" x14ac:dyDescent="0.35">
-      <c r="O69" s="2"/>
+      <c r="O64" s="2"/>
+    </row>
+    <row r="65" spans="15:15" x14ac:dyDescent="0.35">
+      <c r="O65" s="2"/>
     </row>
   </sheetData>
   <dataValidations xWindow="721" yWindow="594" count="12">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Standard deviation" prompt="Enter the standard deviation of the mean of the probability distribution. This cell must be filled only when the selected probability distribution is &quot;Normal&quot;" sqref="K64:K68">
-      <formula1>I64</formula1>
-      <formula2>J64</formula2>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Standard deviation" prompt="Enter the standard deviation of the mean of the probability distribution. This cell must be filled only when the selected probability distribution is &quot;Normal&quot;" sqref="K60:K64">
+      <formula1>I60</formula1>
+      <formula2>J60</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMean" error="Something is wrong. Please enter a value between the minimum and maximum values" promptTitle="Mean" prompt="Enter the most likely value (or mean value) of the probability distribution. This cell must remain empty when the selected probability distribution is &quot;Uniform&quot;_x000a_" sqref="O68">
-      <formula1>K68</formula1>
-      <formula2>L68</formula2>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMean" error="Something is wrong. Please enter a value between the minimum and maximum values" promptTitle="Mean" prompt="Enter the most likely value (or mean value) of the probability distribution. This cell must remain empty when the selected probability distribution is &quot;Uniform&quot;_x000a_" sqref="O64">
+      <formula1>K64</formula1>
+      <formula2>L64</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Standard deviation" prompt="Enter the standard deviation of the mean of the probability distribution. This cell must be filled only when the selected probability distribution is &quot;Normal&quot; or &quot;LogNormal&quot;" sqref="K2:K19 K21:K62">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Standard deviation" prompt="Enter the standard deviation of the mean of the probability distribution. This cell must be filled only when the selected probability distribution is &quot;Normal&quot; or &quot;LogNormal&quot;" sqref="K2:K19 K21:K58">
       <formula1>I2</formula1>
       <formula2>J2</formula2>
     </dataValidation>
@@ -3636,26 +3452,26 @@
       <formula1>O20</formula1>
       <formula2>#REF!</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Other" prompt="Enter the parameter of the probability distribution not covered by the previous columns. Examples: second shape parameter of the Beta distribution_x000a_" sqref="M2:M62"/>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMax" error="Something is wrong. Are you sure the value you entered is the maximal value?" promptTitle="Maximum" prompt="Enter the maximal value of the probability distribution. This cell can be also used to define the upper bound of truncated distributions." sqref="I2:I62">
-      <formula1>H2</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Other" prompt="Enter the parameter of the probability distribution, which had not been covered by the previous columns. Examples: value of the &quot;Point estimate&quot; variable, parameters of &quot;Poisson&quot; or &quot;NegBin&quot; (negative binomial) distributions" sqref="L38:L39 L2:L36 L44:L62"/>
-    <dataValidation type="decimal" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMin" error="Something is wrong. Are you sure the value you entered is the minimum value?" promptTitle="Minimum" prompt="Enter Minimal value of the probability distribution. This cell can be also used to defined the lower bound of truncated distributions." sqref="H2:H62">
-      <formula1>I2</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Other3" prompt="Enter the parameter of the probability distribution not covered by the previous columns. Examples: shift parameter of the shifted log logistic distribution_x000a_" sqref="N2:N62"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Other" prompt="Enter the parameter of the probability distribution, which had not been covered by the previous columns. Examples: value of the &quot;Point estimate&quot; variable, parameters of &quot;Poisson&quot; or &quot;NegBin&quot; (negative binomial) distributions" sqref="L38:L39 L2:L36 L44:L58"/>
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Standard deviation" prompt="Enter the standard deviation of the mean of the probability distribution. This cell must be filled only when the selected probability distribution is &quot;Normal&quot; or &quot;LogNormal&quot;" sqref="L41">
       <formula1>H41</formula1>
       <formula2>I41</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMean" error="Something is wrong. Please enter a value between the minimum and maximum values" promptTitle="Mean" prompt="Enter the most likely value (or mean value) of the probability distribution. _x000a_" sqref="J38:J39 J2:J36 J44:J62">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMean" error="Something is wrong. Please enter a value between the minimum and maximum values" promptTitle="Mean" prompt="Enter the most likely value (or mean value) of the probability distribution. _x000a_" sqref="J38:J39 J2:J36 J44:J58">
       <formula1>H2</formula1>
       <formula2>I2</formula2>
     </dataValidation>
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMean" error="Something is wrong. Please enter a value between the minimum and maximum values" promptTitle="Mean" prompt="Enter the most likely value (or mean value) of the probability distribution. _x000a_" sqref="L42:L43 L40 L37">
       <formula1>H37</formula1>
       <formula2>I37</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Other" prompt="Enter the parameter of the probability distribution not covered by the previous columns. Examples: second shape parameter of the Beta distribution_x000a_" sqref="M2:M58"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Other3" prompt="Enter the parameter of the probability distribution not covered by the previous columns. Examples: shift parameter of the shifted log logistic distribution_x000a_" sqref="N2:N58"/>
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMax" error="Something is wrong. Are you sure the value you entered is the maximal value?" promptTitle="Maximum" prompt="Enter the maximal value of the probability distribution. This cell can be also used to define the upper bound of truncated distributions." sqref="I2:I58">
+      <formula1>H2</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMin" error="Something is wrong. Are you sure the value you entered is the minimum value?" promptTitle="Minimum" prompt="Enter Minimal value of the probability distribution. This cell can be also used to defined the lower bound of truncated distributions." sqref="H2:H58">
+      <formula1>I2</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3667,13 +3483,13 @@
           <x14:formula1>
             <xm:f>ListItem!$B$3:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G62</xm:sqref>
+          <xm:sqref>G2:G58</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Distribution" prompt="Select a probability distribution">
           <x14:formula1>
             <xm:f>ListItem!$A$2:$A$16</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F62</xm:sqref>
+          <xm:sqref>F2:F58</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3699,23 +3515,23 @@
         <v>3</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C1" s="4"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C3" s="2"/>
     </row>
@@ -3724,13 +3540,13 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -3751,63 +3567,63 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>

</xml_diff>

<commit_message>
init. w/ here + farm module integration
</commit_message>
<xml_diff>
--- a/data-input/estimated_variables.xlsx
+++ b/data-input/estimated_variables.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="185">
   <si>
     <t>Module</t>
   </si>
@@ -444,21 +444,6 @@
     <t>Collineau et al. (2020)</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">TODO: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Farm module output</t>
-    </r>
-  </si>
-  <si>
     <t>Prev_wfp_ext.min</t>
   </si>
   <si>
@@ -598,6 +583,12 @@
   </si>
   <si>
     <t>Furusawa et al. (2024)</t>
+  </si>
+  <si>
+    <t>Sarnino et al. (in prep.)</t>
+  </si>
+  <si>
+    <t>Maximum prevalence can be close to 1</t>
   </si>
 </sst>
 </file>
@@ -1159,8 +1150,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="N67" sqref="N67"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1262,7 +1253,7 @@
       </c>
       <c r="N2" s="2"/>
       <c r="O2" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="P2" s="7" t="s">
         <v>125</v>
@@ -1276,10 +1267,10 @@
         <v>94</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D3" s="33" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E3" s="32" t="s">
         <v>102</v>
@@ -1312,10 +1303,10 @@
         <v>94</v>
       </c>
       <c r="C4" s="32" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D4" s="33" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E4" s="32" t="s">
         <v>102</v>
@@ -1331,14 +1322,16 @@
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
       <c r="O4" s="31" t="s">
-        <v>135</v>
-      </c>
-      <c r="P4" s="4"/>
+        <v>183</v>
+      </c>
+      <c r="P4" s="7" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="5" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
@@ -1378,8 +1371,8 @@
       <c r="O5" s="31" t="s">
         <v>135</v>
       </c>
-      <c r="P5" s="4" t="s">
-        <v>136</v>
+      <c r="P5" s="31" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -1418,10 +1411,10 @@
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="P6" s="4" t="s">
-        <v>136</v>
+        <v>152</v>
+      </c>
+      <c r="P6" s="31" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -1534,10 +1527,10 @@
       <c r="M9" s="9"/>
       <c r="N9" s="9"/>
       <c r="O9" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="P9" s="41" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.35">
@@ -1666,10 +1659,10 @@
         <v>94</v>
       </c>
       <c r="C13" s="39" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D13" s="33" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E13" s="32" t="s">
         <v>124</v>
@@ -1702,10 +1695,10 @@
         <v>94</v>
       </c>
       <c r="C14" s="39" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D14" s="33" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E14" s="32" t="s">
         <v>124</v>
@@ -1764,10 +1757,10 @@
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
       <c r="O15" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.35">
@@ -1778,10 +1771,10 @@
         <v>94</v>
       </c>
       <c r="C16" s="32" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D16" s="33" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E16" s="32" t="s">
         <v>10</v>
@@ -1814,10 +1807,10 @@
         <v>94</v>
       </c>
       <c r="C17" s="32" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D17" s="33" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E17" s="32" t="s">
         <v>10</v>
@@ -1856,7 +1849,7 @@
         <v>20</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>5</v>
@@ -1881,7 +1874,7 @@
         <v>135</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.35">
@@ -1998,7 +1991,7 @@
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
       <c r="O21" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.35">
@@ -2077,10 +2070,10 @@
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
       <c r="O23" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="P23" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.35">
@@ -2091,10 +2084,10 @@
         <v>94</v>
       </c>
       <c r="C24" s="32" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D24" s="33" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E24" s="32" t="s">
         <v>10</v>
@@ -2117,7 +2110,7 @@
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
       <c r="O24" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="P24" s="7"/>
     </row>
@@ -2129,13 +2122,13 @@
         <v>94</v>
       </c>
       <c r="C25" s="32" t="s">
+        <v>153</v>
+      </c>
+      <c r="D25" s="33" t="s">
         <v>154</v>
       </c>
-      <c r="D25" s="33" t="s">
-        <v>155</v>
-      </c>
       <c r="E25" s="32" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>5</v>
@@ -2160,7 +2153,7 @@
         <v>135</v>
       </c>
       <c r="P25" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.35">
@@ -2171,13 +2164,13 @@
         <v>94</v>
       </c>
       <c r="C26" s="32" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D26" s="33" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E26" s="32" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>5</v>
@@ -2202,7 +2195,7 @@
         <v>135</v>
       </c>
       <c r="P26" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.35">
@@ -2254,7 +2247,7 @@
         <v>122</v>
       </c>
       <c r="D28" s="33" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E28" s="32" t="s">
         <v>34</v>
@@ -2468,7 +2461,7 @@
         <v>0.25</v>
       </c>
       <c r="O33" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="P33" s="5" t="s">
         <v>118</v>
@@ -2506,7 +2499,7 @@
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
       <c r="O34" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="P34" s="2"/>
     </row>
@@ -2546,7 +2539,7 @@
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
       <c r="O35" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="P35" s="2"/>
     </row>
@@ -2586,7 +2579,7 @@
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
       <c r="O36" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="P36" s="2"/>
     </row>
@@ -2598,10 +2591,10 @@
         <v>94</v>
       </c>
       <c r="C37" s="32" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D37" s="33" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E37" s="32" t="s">
         <v>34</v>
@@ -2657,7 +2650,7 @@
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
       <c r="O38" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="P38" s="2"/>
     </row>
@@ -2693,7 +2686,7 @@
       <c r="M39" s="9"/>
       <c r="N39" s="9"/>
       <c r="O39" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="P39" s="9"/>
     </row>
@@ -2705,7 +2698,7 @@
         <v>60</v>
       </c>
       <c r="C40" s="32" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D40" s="33" t="s">
         <v>113</v>
@@ -2740,10 +2733,10 @@
         <v>60</v>
       </c>
       <c r="C41" s="32" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D41" s="33" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E41" s="32" t="s">
         <v>12</v>
@@ -2775,10 +2768,10 @@
         <v>60</v>
       </c>
       <c r="C42" s="32" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D42" s="33" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E42" s="32" t="s">
         <v>12</v>
@@ -2810,10 +2803,10 @@
         <v>60</v>
       </c>
       <c r="C43" s="32" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D43" s="33" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E43" s="32" t="s">
         <v>12</v>
@@ -3115,7 +3108,7 @@
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
       <c r="O50" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="P50" s="2"/>
     </row>
@@ -3127,10 +3120,10 @@
         <v>60</v>
       </c>
       <c r="C51" s="47" t="s">
+        <v>169</v>
+      </c>
+      <c r="D51" s="48" t="s">
         <v>170</v>
-      </c>
-      <c r="D51" s="48" t="s">
-        <v>171</v>
       </c>
       <c r="E51" s="32" t="s">
         <v>34</v>
@@ -3151,7 +3144,7 @@
       <c r="M51" s="2"/>
       <c r="N51" s="2"/>
       <c r="O51" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="P51" s="2"/>
     </row>
@@ -3163,10 +3156,10 @@
         <v>60</v>
       </c>
       <c r="C52" s="37" t="s">
+        <v>171</v>
+      </c>
+      <c r="D52" s="38" t="s">
         <v>172</v>
-      </c>
-      <c r="D52" s="38" t="s">
-        <v>173</v>
       </c>
       <c r="E52" s="44" t="s">
         <v>34</v>
@@ -3187,7 +3180,7 @@
       <c r="M52" s="5"/>
       <c r="N52" s="5"/>
       <c r="O52" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="P52" s="5"/>
     </row>
@@ -3239,10 +3232,10 @@
         <v>94</v>
       </c>
       <c r="C54" s="32" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D54" s="33" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E54" s="32" t="s">
         <v>10</v>
@@ -3263,7 +3256,7 @@
       <c r="M54" s="2"/>
       <c r="N54" s="2"/>
       <c r="O54" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="P54" s="2"/>
     </row>
@@ -3275,10 +3268,10 @@
         <v>94</v>
       </c>
       <c r="C55" s="32" t="s">
+        <v>180</v>
+      </c>
+      <c r="D55" s="33" t="s">
         <v>181</v>
-      </c>
-      <c r="D55" s="33" t="s">
-        <v>182</v>
       </c>
       <c r="E55" s="32" t="s">
         <v>10</v>
@@ -3299,7 +3292,7 @@
       <c r="M55" s="2"/>
       <c r="N55" s="2"/>
       <c r="O55" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="P55" s="2"/>
     </row>
@@ -3349,10 +3342,10 @@
         <v>60</v>
       </c>
       <c r="C57" s="32" t="s">
+        <v>175</v>
+      </c>
+      <c r="D57" s="33" t="s">
         <v>176</v>
-      </c>
-      <c r="D57" s="33" t="s">
-        <v>177</v>
       </c>
       <c r="E57" s="32" t="s">
         <v>10</v>
@@ -3385,10 +3378,10 @@
         <v>60</v>
       </c>
       <c r="C58" s="32" t="s">
+        <v>177</v>
+      </c>
+      <c r="D58" s="33" t="s">
         <v>178</v>
-      </c>
-      <c r="D58" s="33" t="s">
-        <v>179</v>
       </c>
       <c r="E58" s="32" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Between flock prevalence màj avec Résapath
</commit_message>
<xml_diff>
--- a/data-input/estimated_variables.xlsx
+++ b/data-input/estimated_variables.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="185">
   <si>
     <t>Module</t>
   </si>
@@ -411,9 +411,6 @@
     <t>log10 cfu/ml</t>
   </si>
   <si>
-    <t>assumption: conventional</t>
-  </si>
-  <si>
     <t>OR</t>
   </si>
   <si>
@@ -589,6 +586,9 @@
   </si>
   <si>
     <t>Maximum prevalence can be close to 1</t>
+  </si>
+  <si>
+    <t>Résapath</t>
   </si>
 </sst>
 </file>
@@ -1150,8 +1150,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1159,7 +1159,7 @@
     <col min="1" max="1" width="19.1796875" customWidth="1"/>
     <col min="2" max="2" width="13.54296875" customWidth="1"/>
     <col min="3" max="3" width="18.6328125" customWidth="1"/>
-    <col min="4" max="4" width="25" customWidth="1"/>
+    <col min="4" max="4" width="36.7265625" customWidth="1"/>
     <col min="5" max="5" width="11.7265625" customWidth="1"/>
     <col min="6" max="6" width="14.7265625" customWidth="1"/>
     <col min="7" max="7" width="10.36328125" customWidth="1"/>
@@ -1198,7 +1198,7 @@
         <v>8</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K1" s="8" t="s">
         <v>62</v>
@@ -1236,28 +1236,28 @@
         <v>102</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
+      <c r="H2" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="I2" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="J2" s="2">
+        <v>0.03</v>
+      </c>
       <c r="K2" s="2"/>
-      <c r="L2" s="2">
-        <v>26</v>
-      </c>
-      <c r="M2" s="2">
-        <v>164</v>
-      </c>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
       <c r="N2" s="2"/>
       <c r="O2" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="P2" s="7" t="s">
-        <v>125</v>
-      </c>
+        <v>184</v>
+      </c>
+      <c r="P2" s="7"/>
     </row>
     <row r="3" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="11" t="s">
@@ -1267,10 +1267,10 @@
         <v>94</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D3" s="33" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E3" s="32" t="s">
         <v>102</v>
@@ -1291,7 +1291,7 @@
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
       <c r="O3" s="31" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P3" s="4"/>
     </row>
@@ -1303,10 +1303,10 @@
         <v>94</v>
       </c>
       <c r="C4" s="32" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D4" s="33" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E4" s="32" t="s">
         <v>102</v>
@@ -1327,10 +1327,10 @@
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
       <c r="O4" s="31" t="s">
+        <v>182</v>
+      </c>
+      <c r="P4" s="7" t="s">
         <v>183</v>
-      </c>
-      <c r="P4" s="7" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -1369,10 +1369,10 @@
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="O5" s="31" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P5" s="31" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -1411,10 +1411,10 @@
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="P6" s="31" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -1428,7 +1428,7 @@
         <v>119</v>
       </c>
       <c r="D7" s="33" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E7" s="32" t="s">
         <v>23</v>
@@ -1451,7 +1451,7 @@
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
       <c r="O7" s="31" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P7" s="4"/>
     </row>
@@ -1469,7 +1469,7 @@
         <v>104</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>58</v>
@@ -1487,7 +1487,7 @@
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
       <c r="O8" s="31" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P8" s="4"/>
     </row>
@@ -1527,10 +1527,10 @@
       <c r="M9" s="9"/>
       <c r="N9" s="9"/>
       <c r="O9" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="P9" s="41" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.35">
@@ -1569,7 +1569,7 @@
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
       <c r="O10" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P10" s="2"/>
     </row>
@@ -1607,7 +1607,7 @@
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
       <c r="O11" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P11" s="2"/>
     </row>
@@ -1647,7 +1647,7 @@
       <c r="M12" s="5"/>
       <c r="N12" s="5"/>
       <c r="O12" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P12" s="5"/>
     </row>
@@ -1659,10 +1659,10 @@
         <v>94</v>
       </c>
       <c r="C13" s="39" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D13" s="33" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E13" s="32" t="s">
         <v>124</v>
@@ -1683,7 +1683,7 @@
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
       <c r="O13" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P13" s="2"/>
     </row>
@@ -1695,10 +1695,10 @@
         <v>94</v>
       </c>
       <c r="C14" s="39" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D14" s="33" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E14" s="32" t="s">
         <v>124</v>
@@ -1719,7 +1719,7 @@
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
       <c r="O14" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P14" s="2"/>
     </row>
@@ -1731,10 +1731,10 @@
         <v>94</v>
       </c>
       <c r="C15" s="39" t="s">
+        <v>128</v>
+      </c>
+      <c r="D15" s="40" t="s">
         <v>129</v>
-      </c>
-      <c r="D15" s="40" t="s">
-        <v>130</v>
       </c>
       <c r="E15" s="32" t="s">
         <v>124</v>
@@ -1757,10 +1757,10 @@
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
       <c r="O15" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.35">
@@ -1771,10 +1771,10 @@
         <v>94</v>
       </c>
       <c r="C16" s="32" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D16" s="33" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E16" s="32" t="s">
         <v>10</v>
@@ -1795,7 +1795,7 @@
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
       <c r="O16" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P16" s="2"/>
     </row>
@@ -1807,10 +1807,10 @@
         <v>94</v>
       </c>
       <c r="C17" s="32" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D17" s="33" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E17" s="32" t="s">
         <v>10</v>
@@ -1831,7 +1831,7 @@
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
       <c r="O17" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P17" s="2"/>
     </row>
@@ -1849,7 +1849,7 @@
         <v>20</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>5</v>
@@ -1871,10 +1871,10 @@
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
       <c r="O18" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.35">
@@ -1909,7 +1909,7 @@
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
       <c r="O19" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P19" s="2"/>
     </row>
@@ -1924,7 +1924,7 @@
         <v>24</v>
       </c>
       <c r="D20" s="33" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E20" s="32" t="s">
         <v>23</v>
@@ -1951,7 +1951,7 @@
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
       <c r="O20" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P20" s="3"/>
     </row>
@@ -1991,7 +1991,7 @@
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
       <c r="O21" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.35">
@@ -2030,7 +2030,7 @@
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
       <c r="O22" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P22" s="2"/>
     </row>
@@ -2070,10 +2070,10 @@
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
       <c r="O23" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="P23" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.35">
@@ -2084,10 +2084,10 @@
         <v>94</v>
       </c>
       <c r="C24" s="32" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D24" s="33" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E24" s="32" t="s">
         <v>10</v>
@@ -2110,7 +2110,7 @@
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
       <c r="O24" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="P24" s="7"/>
     </row>
@@ -2122,13 +2122,13 @@
         <v>94</v>
       </c>
       <c r="C25" s="32" t="s">
+        <v>152</v>
+      </c>
+      <c r="D25" s="33" t="s">
         <v>153</v>
       </c>
-      <c r="D25" s="33" t="s">
-        <v>154</v>
-      </c>
       <c r="E25" s="32" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>5</v>
@@ -2150,10 +2150,10 @@
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
       <c r="O25" s="31" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P25" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.35">
@@ -2164,13 +2164,13 @@
         <v>94</v>
       </c>
       <c r="C26" s="32" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D26" s="33" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E26" s="32" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>5</v>
@@ -2192,10 +2192,10 @@
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
       <c r="O26" s="31" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P26" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.35">
@@ -2232,7 +2232,7 @@
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
       <c r="O27" s="31" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P27" s="2"/>
     </row>
@@ -2247,7 +2247,7 @@
         <v>122</v>
       </c>
       <c r="D28" s="33" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E28" s="32" t="s">
         <v>34</v>
@@ -2272,7 +2272,7 @@
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
       <c r="O28" s="31" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P28" s="2"/>
     </row>
@@ -2314,7 +2314,7 @@
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
       <c r="O29" s="31" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P29" s="2"/>
     </row>
@@ -2352,7 +2352,7 @@
       </c>
       <c r="N30" s="9"/>
       <c r="O30" s="46" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P30" s="9"/>
     </row>
@@ -2392,7 +2392,7 @@
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
       <c r="O31" s="31" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P31" s="2"/>
     </row>
@@ -2430,7 +2430,7 @@
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
       <c r="O32" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P32" s="2"/>
     </row>
@@ -2461,7 +2461,7 @@
         <v>0.25</v>
       </c>
       <c r="O33" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="P33" s="5" t="s">
         <v>118</v>
@@ -2499,7 +2499,7 @@
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
       <c r="O34" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="P34" s="2"/>
     </row>
@@ -2539,7 +2539,7 @@
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
       <c r="O35" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="P35" s="2"/>
     </row>
@@ -2579,7 +2579,7 @@
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
       <c r="O36" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="P36" s="2"/>
     </row>
@@ -2591,10 +2591,10 @@
         <v>94</v>
       </c>
       <c r="C37" s="32" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D37" s="33" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E37" s="32" t="s">
         <v>34</v>
@@ -2614,7 +2614,7 @@
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
       <c r="O37" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P37" s="2"/>
     </row>
@@ -2650,7 +2650,7 @@
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
       <c r="O38" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="P38" s="2"/>
     </row>
@@ -2686,7 +2686,7 @@
       <c r="M39" s="9"/>
       <c r="N39" s="9"/>
       <c r="O39" s="10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="P39" s="9"/>
     </row>
@@ -2698,7 +2698,7 @@
         <v>60</v>
       </c>
       <c r="C40" s="32" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D40" s="33" t="s">
         <v>113</v>
@@ -2721,7 +2721,7 @@
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
       <c r="O40" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P40" s="2"/>
     </row>
@@ -2733,10 +2733,10 @@
         <v>60</v>
       </c>
       <c r="C41" s="32" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D41" s="33" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E41" s="32" t="s">
         <v>12</v>
@@ -2756,7 +2756,7 @@
       <c r="M41" s="2"/>
       <c r="N41" s="2"/>
       <c r="O41" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P41" s="2"/>
     </row>
@@ -2768,10 +2768,10 @@
         <v>60</v>
       </c>
       <c r="C42" s="32" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D42" s="33" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E42" s="32" t="s">
         <v>12</v>
@@ -2791,7 +2791,7 @@
       <c r="M42" s="2"/>
       <c r="N42" s="2"/>
       <c r="O42" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P42" s="2"/>
     </row>
@@ -2803,10 +2803,10 @@
         <v>60</v>
       </c>
       <c r="C43" s="32" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D43" s="33" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E43" s="32" t="s">
         <v>12</v>
@@ -2826,7 +2826,7 @@
       <c r="M43" s="2"/>
       <c r="N43" s="2"/>
       <c r="O43" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P43" s="2"/>
     </row>
@@ -2864,7 +2864,7 @@
       <c r="M44" s="2"/>
       <c r="N44" s="2"/>
       <c r="O44" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P44" s="2"/>
     </row>
@@ -2904,7 +2904,7 @@
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
       <c r="O45" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P45" s="2"/>
     </row>
@@ -2919,7 +2919,7 @@
         <v>43</v>
       </c>
       <c r="D46" s="33" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E46" s="32" t="s">
         <v>44</v>
@@ -2942,7 +2942,7 @@
       <c r="M46" s="2"/>
       <c r="N46" s="2"/>
       <c r="O46" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P46" s="2"/>
     </row>
@@ -2957,7 +2957,7 @@
         <v>47</v>
       </c>
       <c r="D47" s="33" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E47" s="32" t="s">
         <v>39</v>
@@ -2980,7 +2980,7 @@
       <c r="M47" s="2"/>
       <c r="N47" s="2"/>
       <c r="O47" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P47" s="2"/>
     </row>
@@ -3022,7 +3022,7 @@
       <c r="M48" s="2"/>
       <c r="N48" s="2"/>
       <c r="O48" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P48" s="2"/>
     </row>
@@ -3066,7 +3066,7 @@
         <v>-22.914999999999999</v>
       </c>
       <c r="O49" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P49" s="2"/>
     </row>
@@ -3108,7 +3108,7 @@
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
       <c r="O50" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="P50" s="2"/>
     </row>
@@ -3120,10 +3120,10 @@
         <v>60</v>
       </c>
       <c r="C51" s="47" t="s">
+        <v>168</v>
+      </c>
+      <c r="D51" s="48" t="s">
         <v>169</v>
-      </c>
-      <c r="D51" s="48" t="s">
-        <v>170</v>
       </c>
       <c r="E51" s="32" t="s">
         <v>34</v>
@@ -3144,7 +3144,7 @@
       <c r="M51" s="2"/>
       <c r="N51" s="2"/>
       <c r="O51" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="P51" s="2"/>
     </row>
@@ -3156,10 +3156,10 @@
         <v>60</v>
       </c>
       <c r="C52" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="D52" s="38" t="s">
         <v>171</v>
-      </c>
-      <c r="D52" s="38" t="s">
-        <v>172</v>
       </c>
       <c r="E52" s="44" t="s">
         <v>34</v>
@@ -3180,7 +3180,7 @@
       <c r="M52" s="5"/>
       <c r="N52" s="5"/>
       <c r="O52" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="P52" s="5"/>
     </row>
@@ -3220,7 +3220,7 @@
       <c r="M53" s="2"/>
       <c r="N53" s="2"/>
       <c r="O53" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P53" s="2"/>
     </row>
@@ -3232,10 +3232,10 @@
         <v>94</v>
       </c>
       <c r="C54" s="32" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D54" s="33" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E54" s="32" t="s">
         <v>10</v>
@@ -3256,7 +3256,7 @@
       <c r="M54" s="2"/>
       <c r="N54" s="2"/>
       <c r="O54" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="P54" s="2"/>
     </row>
@@ -3268,10 +3268,10 @@
         <v>94</v>
       </c>
       <c r="C55" s="32" t="s">
+        <v>179</v>
+      </c>
+      <c r="D55" s="33" t="s">
         <v>180</v>
-      </c>
-      <c r="D55" s="33" t="s">
-        <v>181</v>
       </c>
       <c r="E55" s="32" t="s">
         <v>10</v>
@@ -3292,7 +3292,7 @@
       <c r="M55" s="2"/>
       <c r="N55" s="2"/>
       <c r="O55" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="P55" s="2"/>
     </row>
@@ -3307,7 +3307,7 @@
         <v>51</v>
       </c>
       <c r="D56" s="33" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E56" s="32" t="s">
         <v>23</v>
@@ -3330,7 +3330,7 @@
       <c r="M56" s="2"/>
       <c r="N56" s="2"/>
       <c r="O56" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P56" s="2"/>
     </row>
@@ -3342,10 +3342,10 @@
         <v>60</v>
       </c>
       <c r="C57" s="32" t="s">
+        <v>174</v>
+      </c>
+      <c r="D57" s="33" t="s">
         <v>175</v>
-      </c>
-      <c r="D57" s="33" t="s">
-        <v>176</v>
       </c>
       <c r="E57" s="32" t="s">
         <v>10</v>
@@ -3366,7 +3366,7 @@
       <c r="M57" s="2"/>
       <c r="N57" s="2"/>
       <c r="O57" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P57" s="2"/>
     </row>
@@ -3378,10 +3378,10 @@
         <v>60</v>
       </c>
       <c r="C58" s="32" t="s">
+        <v>176</v>
+      </c>
+      <c r="D58" s="33" t="s">
         <v>177</v>
-      </c>
-      <c r="D58" s="33" t="s">
-        <v>178</v>
       </c>
       <c r="E58" s="32" t="s">
         <v>10</v>
@@ -3402,7 +3402,7 @@
       <c r="M58" s="2"/>
       <c r="N58" s="2"/>
       <c r="O58" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P58" s="2"/>
     </row>
@@ -3442,7 +3442,7 @@
       <c r="M59" s="2"/>
       <c r="N59" s="2"/>
       <c r="O59" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P59" s="2"/>
     </row>
@@ -3482,7 +3482,7 @@
       <c r="M60" s="2"/>
       <c r="N60" s="2"/>
       <c r="O60" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P60" s="2"/>
     </row>

</xml_diff>